<commit_message>
cleanup draft dsd for syb
</commit_message>
<xml_diff>
--- a/unsd/UNSYB/data/SYB series mapping to DSD.xlsx
+++ b/unsd/UNSYB/data/SYB series mapping to DSD.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\unsd\UNSYB\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85F83497-C045-4615-83E3-C7082862CACB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47465C14-E75E-4336-9394-1D04C6CE6A0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ref_series_df" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="622">
   <si>
     <t>seriesCode</t>
   </si>
@@ -1318,9 +1318,6 @@
     <t>Balance of Payments: Financial account</t>
   </si>
   <si>
-    <t>International traffic - passenger-kilometres</t>
-  </si>
-  <si>
     <t>International traffic - passengers carried</t>
   </si>
   <si>
@@ -1363,9 +1360,6 @@
     <t>Total traffic - passenger-distance</t>
   </si>
   <si>
-    <t>Tons</t>
-  </si>
-  <si>
     <t>Proportion of population with access to safely managed sanitation facilities</t>
   </si>
   <si>
@@ -1459,9 +1453,6 @@
     <t>Number of deaths per 1,000 live births</t>
   </si>
   <si>
-    <t xml:space="preserve">MALES </t>
-  </si>
-  <si>
     <t>Infant mortality ratio</t>
   </si>
   <si>
@@ -1588,9 +1579,6 @@
     <t>International maritime transport: Vessels entered</t>
   </si>
   <si>
-    <t>Total traffic - distance distance</t>
-  </si>
-  <si>
     <t>International traffic - total weight-distance</t>
   </si>
   <si>
@@ -1654,9 +1642,6 @@
     <t>Technicians</t>
   </si>
   <si>
-    <t>WOMEN</t>
-  </si>
-  <si>
     <t>Balance imports/exports</t>
   </si>
   <si>
@@ -1672,12 +1657,6 @@
     <t>Balance of Payments: Current account</t>
   </si>
   <si>
-    <t>Exchange rates: end of period</t>
-  </si>
-  <si>
-    <t>Exchange rates: period average</t>
-  </si>
-  <si>
     <t>Asylum seekers, including pending cases</t>
   </si>
   <si>
@@ -1807,9 +1786,6 @@
     <t>Pre-primary</t>
   </si>
   <si>
-    <t>Public expenditure in education</t>
-  </si>
-  <si>
     <t>Percent of GDP</t>
   </si>
   <si>
@@ -1837,9 +1813,6 @@
     <t>Pupil to teacher ratio</t>
   </si>
   <si>
-    <t>Tertiatry</t>
-  </si>
-  <si>
     <t>Number of teachers</t>
   </si>
   <si>
@@ -1871,12 +1844,57 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>International traffic - passenger-distance</t>
+  </si>
+  <si>
+    <t>Health personnel per 1000 population</t>
+  </si>
+  <si>
+    <t>Carbon dioxide emissions per capita</t>
+  </si>
+  <si>
+    <t>Public expenditure in education as percent of GDP</t>
+  </si>
+  <si>
+    <t>Public expenditure in education as percent of government expenditure</t>
+  </si>
+  <si>
+    <t>Net official development assistance to developing countries and multilateral organizations as percent of GNI</t>
+  </si>
+  <si>
+    <t>International migrant stock as percent of total population</t>
+  </si>
+  <si>
+    <t>Exchange rate: end of period</t>
+  </si>
+  <si>
+    <t>Exchange rate: period average</t>
+  </si>
+  <si>
+    <t>Net official development assistance received as percent of GNI</t>
+  </si>
+  <si>
+    <t>Permanent crops as percent of total land area</t>
+  </si>
+  <si>
+    <t>Important sites for terrestrial biodiversity protected as percent of total sites protected</t>
+  </si>
+  <si>
+    <t>Forest cover as percent of total land area</t>
+  </si>
+  <si>
+    <t>Arable land as percent of total land area</t>
+  </si>
+  <si>
+    <t>Total traffic - distance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2724,14 +2742,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,7 +2765,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2774,25 +2792,25 @@
         <v>414</v>
       </c>
       <c r="J1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="K1" t="s">
         <v>425</v>
       </c>
       <c r="L1" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="M1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="N1" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="O1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="P1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="Q1" t="s">
         <v>412</v>
@@ -2801,7 +2819,7 @@
         <v>416</v>
       </c>
       <c r="S1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T1" t="s">
         <v>417</v>
@@ -2824,16 +2842,16 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="T2" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -2853,16 +2871,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="T3" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -2882,16 +2900,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I4" t="s">
+        <v>451</v>
+      </c>
+      <c r="S4" t="s">
+        <v>459</v>
+      </c>
+      <c r="T4" t="s">
         <v>453</v>
-      </c>
-      <c r="S4" t="s">
-        <v>461</v>
-      </c>
-      <c r="T4" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
@@ -2911,16 +2929,16 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I5" t="s">
+        <v>451</v>
+      </c>
+      <c r="S5" t="s">
+        <v>458</v>
+      </c>
+      <c r="T5" t="s">
         <v>453</v>
-      </c>
-      <c r="S5" t="s">
-        <v>460</v>
-      </c>
-      <c r="T5" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
@@ -2940,16 +2958,16 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="T6" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -2969,16 +2987,16 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I7" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="S7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="T7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -2998,7 +3016,7 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I8" t="s">
         <v>424</v>
@@ -3007,10 +3025,10 @@
         <v>3</v>
       </c>
       <c r="S8" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T8" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -3030,7 +3048,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I9" t="s">
         <v>424</v>
@@ -3039,10 +3057,10 @@
         <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3062,7 +3080,7 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I10" t="s">
         <v>424</v>
@@ -3071,10 +3089,10 @@
         <v>3</v>
       </c>
       <c r="S10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="T10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -3094,13 +3112,13 @@
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I11" t="s">
         <v>424</v>
       </c>
       <c r="O11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -3120,13 +3138,13 @@
         <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I12" t="s">
         <v>424</v>
       </c>
       <c r="O12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -3146,7 +3164,7 @@
         <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I13" t="s">
         <v>424</v>
@@ -3172,7 +3190,7 @@
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I14" t="s">
         <v>424</v>
@@ -3198,7 +3216,7 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I15" t="s">
         <v>415</v>
@@ -3221,7 +3239,7 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I16" t="s">
         <v>415</v>
@@ -3244,7 +3262,7 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I17" t="s">
         <v>415</v>
@@ -3267,7 +3285,7 @@
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I18" t="s">
         <v>415</v>
@@ -3290,7 +3308,7 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I19" t="s">
         <v>415</v>
@@ -3313,7 +3331,7 @@
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I20" t="s">
         <v>415</v>
@@ -3336,7 +3354,7 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I21" t="s">
         <v>415</v>
@@ -3359,13 +3377,13 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="I22" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="S22" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -3385,13 +3403,13 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
+        <v>438</v>
+      </c>
+      <c r="I23" t="s">
         <v>439</v>
       </c>
-      <c r="I23" t="s">
-        <v>440</v>
-      </c>
       <c r="S23" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -3411,13 +3429,13 @@
         <v>8</v>
       </c>
       <c r="H24" t="s">
+        <v>438</v>
+      </c>
+      <c r="I24" t="s">
         <v>439</v>
       </c>
-      <c r="I24" t="s">
-        <v>440</v>
-      </c>
       <c r="S24" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -3437,13 +3455,13 @@
         <v>8</v>
       </c>
       <c r="H25" t="s">
+        <v>438</v>
+      </c>
+      <c r="I25" t="s">
         <v>439</v>
       </c>
-      <c r="I25" t="s">
-        <v>440</v>
-      </c>
       <c r="S25" t="s">
-        <v>478</v>
+        <v>458</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -3463,10 +3481,10 @@
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I26" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -3509,10 +3527,10 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I28" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
@@ -3673,7 +3691,7 @@
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>296</v>
@@ -3691,18 +3709,18 @@
         <v>18</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>298</v>
@@ -3720,18 +3738,18 @@
         <v>18</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>300</v>
@@ -3749,13 +3767,13 @@
         <v>18</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -3775,10 +3793,10 @@
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="I38" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J38">
         <v>6</v>
@@ -3804,10 +3822,10 @@
         <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I39" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J39">
         <v>6</v>
@@ -3830,10 +3848,10 @@
         <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="I40" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -3853,7 +3871,7 @@
         <v>19</v>
       </c>
       <c r="H41" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="I41" t="s">
         <v>415</v>
@@ -3876,16 +3894,16 @@
         <v>23</v>
       </c>
       <c r="H42" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I42" t="s">
         <v>428</v>
       </c>
       <c r="K42" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N42" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -3905,16 +3923,16 @@
         <v>23</v>
       </c>
       <c r="H43" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I43" t="s">
         <v>428</v>
       </c>
       <c r="K43" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N43" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -3934,16 +3952,16 @@
         <v>23</v>
       </c>
       <c r="H44" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I44" t="s">
         <v>428</v>
       </c>
       <c r="K44" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N44" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3963,16 +3981,16 @@
         <v>23</v>
       </c>
       <c r="H45" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I45" t="s">
         <v>428</v>
       </c>
       <c r="K45" t="s">
+        <v>488</v>
+      </c>
+      <c r="N45" t="s">
         <v>491</v>
-      </c>
-      <c r="N45" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -3992,16 +4010,16 @@
         <v>23</v>
       </c>
       <c r="H46" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I46" t="s">
         <v>428</v>
       </c>
       <c r="K46" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N46" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -4021,16 +4039,16 @@
         <v>23</v>
       </c>
       <c r="H47" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I47" t="s">
         <v>428</v>
       </c>
       <c r="K47" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N47" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -4050,16 +4068,16 @@
         <v>23</v>
       </c>
       <c r="H48" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I48" t="s">
         <v>428</v>
       </c>
       <c r="K48" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N48" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
@@ -4079,16 +4097,16 @@
         <v>23</v>
       </c>
       <c r="H49" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I49" t="s">
         <v>428</v>
       </c>
       <c r="K49" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N49" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.25">
@@ -4108,16 +4126,16 @@
         <v>23</v>
       </c>
       <c r="H50" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I50" t="s">
         <v>428</v>
       </c>
       <c r="K50" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N50" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
@@ -4137,16 +4155,16 @@
         <v>23</v>
       </c>
       <c r="H51" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I51" t="s">
         <v>428</v>
       </c>
       <c r="K51" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N51" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
@@ -4166,16 +4184,16 @@
         <v>23</v>
       </c>
       <c r="H52" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I52" t="s">
         <v>428</v>
       </c>
       <c r="K52" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N52" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
@@ -4195,16 +4213,16 @@
         <v>23</v>
       </c>
       <c r="H53" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I53" t="s">
         <v>428</v>
       </c>
       <c r="K53" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N53" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.25">
@@ -4224,16 +4242,16 @@
         <v>23</v>
       </c>
       <c r="H54" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I54" t="s">
         <v>428</v>
       </c>
       <c r="K54" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N54" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.25">
@@ -4253,16 +4271,16 @@
         <v>23</v>
       </c>
       <c r="H55" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I55" t="s">
         <v>428</v>
       </c>
       <c r="K55" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N55" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.25">
@@ -4282,16 +4300,16 @@
         <v>23</v>
       </c>
       <c r="H56" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="I56" t="s">
         <v>428</v>
       </c>
       <c r="K56" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="N56" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
@@ -4311,7 +4329,7 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="I57" t="s">
         <v>428</v>
@@ -4337,7 +4355,7 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="I58" t="s">
         <v>428</v>
@@ -4363,16 +4381,16 @@
         <v>49</v>
       </c>
       <c r="H59" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I59" t="s">
         <v>415</v>
       </c>
       <c r="N59" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="S59" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
@@ -4392,16 +4410,16 @@
         <v>49</v>
       </c>
       <c r="H60" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I60" t="s">
         <v>415</v>
       </c>
       <c r="N60" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="S60" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
@@ -4421,16 +4439,16 @@
         <v>49</v>
       </c>
       <c r="H61" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I61" t="s">
         <v>415</v>
       </c>
       <c r="N61" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="S61" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="62" spans="2:19" x14ac:dyDescent="0.25">
@@ -4450,16 +4468,16 @@
         <v>49</v>
       </c>
       <c r="H62" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I62" t="s">
         <v>415</v>
       </c>
       <c r="N62" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="S62" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
@@ -4479,16 +4497,16 @@
         <v>49</v>
       </c>
       <c r="H63" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I63" t="s">
         <v>415</v>
       </c>
       <c r="N63" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="S63" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="64" spans="2:19" x14ac:dyDescent="0.25">
@@ -4508,16 +4526,16 @@
         <v>49</v>
       </c>
       <c r="H64" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I64" t="s">
         <v>415</v>
       </c>
       <c r="N64" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="S64" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.25">
@@ -4537,16 +4555,16 @@
         <v>49</v>
       </c>
       <c r="H65" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I65" t="s">
         <v>415</v>
       </c>
       <c r="N65" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="S65" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="66" spans="2:19" x14ac:dyDescent="0.25">
@@ -4566,16 +4584,16 @@
         <v>49</v>
       </c>
       <c r="H66" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I66" t="s">
         <v>415</v>
       </c>
       <c r="N66" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="S66" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.25">
@@ -4595,16 +4613,16 @@
         <v>49</v>
       </c>
       <c r="H67" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="I67" t="s">
         <v>415</v>
       </c>
       <c r="N67" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="S67" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
@@ -4624,10 +4642,10 @@
         <v>57</v>
       </c>
       <c r="H68" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I68" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J68">
         <v>6</v>
@@ -4650,10 +4668,10 @@
         <v>57</v>
       </c>
       <c r="H69" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="I69" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="J69">
         <v>6</v>
@@ -4676,10 +4694,10 @@
         <v>58</v>
       </c>
       <c r="H70" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="I70" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="J70">
         <v>3</v>
@@ -4702,10 +4720,10 @@
         <v>58</v>
       </c>
       <c r="H71" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I71" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="J71">
         <v>3</v>
@@ -4728,10 +4746,10 @@
         <v>60</v>
       </c>
       <c r="H72" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I72" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="J72">
         <v>3</v>
@@ -4754,10 +4772,10 @@
         <v>60</v>
       </c>
       <c r="H73" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I73" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="J73">
         <v>3</v>
@@ -4780,10 +4798,10 @@
         <v>61</v>
       </c>
       <c r="H74" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I74" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J74">
         <v>6</v>
@@ -4806,10 +4824,10 @@
         <v>61</v>
       </c>
       <c r="H75" t="s">
-        <v>431</v>
+        <v>607</v>
       </c>
       <c r="I75" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="J75">
         <v>6</v>
@@ -4832,10 +4850,10 @@
         <v>61</v>
       </c>
       <c r="H76" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I76" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="J76">
         <v>3</v>
@@ -4858,10 +4876,10 @@
         <v>61</v>
       </c>
       <c r="H77" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="I77" t="s">
-        <v>446</v>
+        <v>506</v>
       </c>
       <c r="J77">
         <v>6</v>
@@ -4884,10 +4902,10 @@
         <v>61</v>
       </c>
       <c r="H78" t="s">
-        <v>521</v>
+        <v>621</v>
       </c>
       <c r="I78" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="J78">
         <v>6</v>
@@ -4910,10 +4928,10 @@
         <v>61</v>
       </c>
       <c r="H79" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I79" t="s">
-        <v>443</v>
+        <v>507</v>
       </c>
       <c r="J79">
         <v>6</v>
@@ -4936,10 +4954,10 @@
         <v>61</v>
       </c>
       <c r="H80" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="I80" t="s">
-        <v>424</v>
+        <v>509</v>
       </c>
       <c r="J80">
         <v>3</v>
@@ -4962,10 +4980,10 @@
         <v>61</v>
       </c>
       <c r="H81" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I81" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="J81">
         <v>6</v>
@@ -4988,7 +5006,7 @@
         <v>64</v>
       </c>
       <c r="H82" t="s">
-        <v>287</v>
+        <v>620</v>
       </c>
       <c r="I82" t="s">
         <v>415</v>
@@ -5011,10 +5029,10 @@
         <v>64</v>
       </c>
       <c r="H83" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I83" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="J83">
         <v>3</v>
@@ -5037,7 +5055,7 @@
         <v>64</v>
       </c>
       <c r="H84" t="s">
-        <v>291</v>
+        <v>619</v>
       </c>
       <c r="I84" t="s">
         <v>415</v>
@@ -5060,10 +5078,10 @@
         <v>64</v>
       </c>
       <c r="H85" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="I85" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="J85">
         <v>3</v>
@@ -5086,7 +5104,7 @@
         <v>64</v>
       </c>
       <c r="H86" t="s">
-        <v>47</v>
+        <v>618</v>
       </c>
       <c r="I86" t="s">
         <v>415</v>
@@ -5094,7 +5112,7 @@
     </row>
     <row r="87" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>204</v>
@@ -5112,10 +5130,10 @@
         <v>64</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="J87" s="1">
         <v>3</v>
@@ -5138,7 +5156,7 @@
         <v>64</v>
       </c>
       <c r="H88" t="s">
-        <v>289</v>
+        <v>617</v>
       </c>
       <c r="I88" t="s">
         <v>415</v>
@@ -5161,10 +5179,10 @@
         <v>64</v>
       </c>
       <c r="H89" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="I89" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="J89">
         <v>3</v>
@@ -5187,10 +5205,10 @@
         <v>65</v>
       </c>
       <c r="H90" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="I90" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
@@ -5210,10 +5228,10 @@
         <v>65</v>
       </c>
       <c r="H91" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="I91" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -5233,10 +5251,10 @@
         <v>65</v>
       </c>
       <c r="H92" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="I92" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
@@ -5256,10 +5274,10 @@
         <v>65</v>
       </c>
       <c r="H93" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="I93" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
@@ -5279,10 +5297,10 @@
         <v>65</v>
       </c>
       <c r="H94" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="I94" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -5302,16 +5320,16 @@
         <v>66</v>
       </c>
       <c r="H95" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="I95" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="M95" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="S95" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -5331,16 +5349,16 @@
         <v>66</v>
       </c>
       <c r="H96" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="I96" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="M96" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="S96" t="s">
-        <v>543</v>
+        <v>459</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
@@ -5360,16 +5378,16 @@
         <v>66</v>
       </c>
       <c r="H97" t="s">
+        <v>533</v>
+      </c>
+      <c r="I97" t="s">
+        <v>535</v>
+      </c>
+      <c r="M97" t="s">
         <v>537</v>
       </c>
-      <c r="I97" t="s">
-        <v>539</v>
-      </c>
-      <c r="M97" t="s">
-        <v>541</v>
-      </c>
       <c r="S97" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
@@ -5389,16 +5407,16 @@
         <v>66</v>
       </c>
       <c r="H98" t="s">
+        <v>533</v>
+      </c>
+      <c r="I98" t="s">
+        <v>535</v>
+      </c>
+      <c r="M98" t="s">
         <v>537</v>
       </c>
-      <c r="I98" t="s">
-        <v>539</v>
-      </c>
-      <c r="M98" t="s">
-        <v>541</v>
-      </c>
       <c r="S98" t="s">
-        <v>543</v>
+        <v>459</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
@@ -5418,16 +5436,16 @@
         <v>66</v>
       </c>
       <c r="H99" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="I99" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="M99" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="S99" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
@@ -5447,16 +5465,16 @@
         <v>66</v>
       </c>
       <c r="H100" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="I100" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="M100" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="S100" t="s">
-        <v>543</v>
+        <v>459</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
@@ -5476,16 +5494,16 @@
         <v>66</v>
       </c>
       <c r="H101" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="I101" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="M101" t="s">
         <v>422</v>
       </c>
       <c r="S101" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
@@ -5505,7 +5523,7 @@
         <v>67</v>
       </c>
       <c r="H102" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="I102" t="s">
         <v>424</v>
@@ -5528,7 +5546,7 @@
         <v>67</v>
       </c>
       <c r="H103" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="I103" t="s">
         <v>424</v>
@@ -5551,15 +5569,15 @@
         <v>67</v>
       </c>
       <c r="H104" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="I104" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
     </row>
     <row r="105" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>202</v>
@@ -5580,10 +5598,10 @@
         <v>68</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J105" s="1">
         <v>6</v>
@@ -5591,7 +5609,7 @@
     </row>
     <row r="106" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>96</v>
@@ -5612,10 +5630,10 @@
         <v>68</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J106" s="1">
         <v>6</v>
@@ -5623,7 +5641,7 @@
     </row>
     <row r="107" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>120</v>
@@ -5644,10 +5662,10 @@
         <v>68</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J107" s="1">
         <v>6</v>
@@ -5655,7 +5673,7 @@
     </row>
     <row r="108" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>216</v>
@@ -5673,10 +5691,10 @@
         <v>74</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J108" s="1">
         <v>6</v>
@@ -5684,7 +5702,7 @@
     </row>
     <row r="109" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>214</v>
@@ -5702,10 +5720,10 @@
         <v>74</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J109" s="1">
         <v>6</v>
@@ -5713,7 +5731,7 @@
     </row>
     <row r="110" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>32</v>
@@ -5734,7 +5752,7 @@
         <v>430</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J110" s="1">
         <v>6</v>
@@ -5742,7 +5760,7 @@
     </row>
     <row r="111" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>92</v>
@@ -5763,15 +5781,15 @@
         <v>75</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>549</v>
+        <v>614</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="112" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>94</v>
@@ -5792,10 +5810,10 @@
         <v>75</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>550</v>
+        <v>615</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
@@ -5815,16 +5833,16 @@
         <v>77</v>
       </c>
       <c r="H113" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I113" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J113">
         <v>6</v>
       </c>
       <c r="K113" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
@@ -5844,16 +5862,16 @@
         <v>77</v>
       </c>
       <c r="H114" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I114" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J114">
         <v>6</v>
       </c>
       <c r="K114" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
@@ -5873,10 +5891,10 @@
         <v>77</v>
       </c>
       <c r="H115" t="s">
-        <v>449</v>
+        <v>616</v>
       </c>
       <c r="I115" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="K115" t="s">
         <v>422</v>
@@ -5899,10 +5917,10 @@
         <v>77</v>
       </c>
       <c r="H116" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I116" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J116">
         <v>6</v>
@@ -5928,7 +5946,7 @@
         <v>78</v>
       </c>
       <c r="H117" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="I117" t="s">
         <v>424</v>
@@ -5936,7 +5954,7 @@
     </row>
     <row r="118" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>354</v>
@@ -5954,18 +5972,18 @@
         <v>78</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>567</v>
+        <v>613</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="119" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>350</v>
@@ -5983,18 +6001,18 @@
         <v>78</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>424</v>
       </c>
       <c r="S119" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="120" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>358</v>
@@ -6012,18 +6030,18 @@
         <v>78</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>567</v>
+        <v>613</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="121" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>356</v>
@@ -6041,18 +6059,18 @@
         <v>78</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>567</v>
+        <v>613</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="122" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>362</v>
@@ -6070,7 +6088,7 @@
         <v>78</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>424</v>
@@ -6078,7 +6096,7 @@
     </row>
     <row r="123" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>364</v>
@@ -6096,7 +6114,7 @@
         <v>78</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>424</v>
@@ -6104,7 +6122,7 @@
     </row>
     <row r="124" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>352</v>
@@ -6122,7 +6140,7 @@
         <v>78</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>424</v>
@@ -6130,7 +6148,7 @@
     </row>
     <row r="125" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>154</v>
@@ -6151,15 +6169,15 @@
         <v>83</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
     </row>
     <row r="126" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>156</v>
@@ -6180,15 +6198,15 @@
         <v>83</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
     </row>
     <row r="127" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>152</v>
@@ -6209,7 +6227,7 @@
         <v>83</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="I127" s="1" t="s">
         <v>424</v>
@@ -6220,7 +6238,7 @@
     </row>
     <row r="128" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>172</v>
@@ -6238,7 +6256,7 @@
         <v>83</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>415</v>
@@ -6249,7 +6267,7 @@
     </row>
     <row r="129" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>174</v>
@@ -6267,7 +6285,7 @@
         <v>83</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>415</v>
@@ -6278,7 +6296,7 @@
     </row>
     <row r="130" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>170</v>
@@ -6296,10 +6314,10 @@
         <v>83</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="Q130" s="1" t="s">
         <v>420</v>
@@ -6556,7 +6574,7 @@
         <v>84</v>
       </c>
       <c r="H140" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I140" t="s">
         <v>415</v>
@@ -6582,7 +6600,7 @@
         <v>84</v>
       </c>
       <c r="H141" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I141" t="s">
         <v>415</v>
@@ -6608,7 +6626,7 @@
         <v>84</v>
       </c>
       <c r="H142" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I142" t="s">
         <v>415</v>
@@ -6619,7 +6637,7 @@
     </row>
     <row r="143" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>38</v>
@@ -6637,18 +6655,18 @@
         <v>89</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>415</v>
       </c>
       <c r="R143" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="144" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>40</v>
@@ -6666,18 +6684,18 @@
         <v>89</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>415</v>
       </c>
       <c r="R144" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="145" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>212</v>
@@ -6700,7 +6718,7 @@
     </row>
     <row r="146" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>208</v>
@@ -6718,7 +6736,7 @@
         <v>89</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>424</v>
@@ -6727,12 +6745,12 @@
         <v>6</v>
       </c>
       <c r="S146" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="147" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>88</v>
@@ -6750,7 +6768,7 @@
         <v>89</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>424</v>
@@ -6759,12 +6777,12 @@
         <v>6</v>
       </c>
       <c r="S147" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="148" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>90</v>
@@ -6782,7 +6800,7 @@
         <v>89</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>424</v>
@@ -6791,12 +6809,12 @@
         <v>6</v>
       </c>
       <c r="S148" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="149" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>42</v>
@@ -6822,7 +6840,7 @@
     </row>
     <row r="150" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>210</v>
@@ -6840,10 +6858,10 @@
         <v>89</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="J150" s="1">
         <v>3</v>
@@ -6866,13 +6884,13 @@
         <v>94</v>
       </c>
       <c r="H151" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="I151" t="s">
         <v>415</v>
       </c>
       <c r="S151" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="152" spans="1:19" x14ac:dyDescent="0.25">
@@ -6892,13 +6910,13 @@
         <v>94</v>
       </c>
       <c r="H152" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="I152" t="s">
         <v>415</v>
       </c>
       <c r="S152" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="153" spans="1:19" x14ac:dyDescent="0.25">
@@ -6918,13 +6936,13 @@
         <v>94</v>
       </c>
       <c r="H153" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="I153" t="s">
         <v>415</v>
       </c>
       <c r="S153" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="154" spans="1:19" x14ac:dyDescent="0.25">
@@ -6944,13 +6962,13 @@
         <v>94</v>
       </c>
       <c r="H154" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="I154" t="s">
         <v>415</v>
       </c>
       <c r="S154" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="155" spans="1:19" x14ac:dyDescent="0.25">
@@ -6970,13 +6988,13 @@
         <v>94</v>
       </c>
       <c r="H155" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="I155" t="s">
         <v>415</v>
       </c>
       <c r="S155" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="156" spans="1:19" x14ac:dyDescent="0.25">
@@ -6996,18 +7014,18 @@
         <v>94</v>
       </c>
       <c r="H156" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="I156" t="s">
         <v>415</v>
       </c>
       <c r="S156" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="157" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>342</v>
@@ -7025,7 +7043,7 @@
         <v>98</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="I157" s="1" t="s">
         <v>428</v>
@@ -7033,7 +7051,7 @@
     </row>
     <row r="158" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>344</v>
@@ -7051,7 +7069,7 @@
         <v>98</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="I158" s="1" t="s">
         <v>428</v>
@@ -7074,10 +7092,10 @@
         <v>103</v>
       </c>
       <c r="H159" t="s">
-        <v>347</v>
+        <v>612</v>
       </c>
       <c r="I159" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
     </row>
     <row r="160" spans="1:19" x14ac:dyDescent="0.25">
@@ -7097,10 +7115,10 @@
         <v>103</v>
       </c>
       <c r="H160" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="I160" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J160">
         <v>6</v>
@@ -7123,10 +7141,10 @@
         <v>104</v>
       </c>
       <c r="H161" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="I161" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="162" spans="2:20" x14ac:dyDescent="0.25">
@@ -7146,10 +7164,10 @@
         <v>104</v>
       </c>
       <c r="H162" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="I162" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="163" spans="2:20" x14ac:dyDescent="0.25">
@@ -7169,10 +7187,10 @@
         <v>104</v>
       </c>
       <c r="H163" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="I163" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="164" spans="2:20" x14ac:dyDescent="0.25">
@@ -7192,13 +7210,13 @@
         <v>104</v>
       </c>
       <c r="H164" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="I164" t="s">
         <v>415</v>
       </c>
       <c r="S164" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="165" spans="2:20" x14ac:dyDescent="0.25">
@@ -7218,13 +7236,13 @@
         <v>104</v>
       </c>
       <c r="H165" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="I165" t="s">
         <v>415</v>
       </c>
       <c r="S165" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="166" spans="2:20" x14ac:dyDescent="0.25">
@@ -7244,10 +7262,10 @@
         <v>104</v>
       </c>
       <c r="H166" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="I166" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="167" spans="2:20" x14ac:dyDescent="0.25">
@@ -7267,10 +7285,10 @@
         <v>104</v>
       </c>
       <c r="H167" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="I167" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="168" spans="2:20" x14ac:dyDescent="0.25">
@@ -7290,10 +7308,10 @@
         <v>104</v>
       </c>
       <c r="H168" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="I168" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
     </row>
     <row r="169" spans="2:20" x14ac:dyDescent="0.25">
@@ -7336,7 +7354,7 @@
         <v>107</v>
       </c>
       <c r="H170" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="I170" t="s">
         <v>424</v>
@@ -7359,10 +7377,10 @@
         <v>107</v>
       </c>
       <c r="H171" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="I171" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
     </row>
     <row r="172" spans="2:20" x14ac:dyDescent="0.25">
@@ -7382,13 +7400,13 @@
         <v>109</v>
       </c>
       <c r="H172" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="I172" t="s">
         <v>415</v>
       </c>
       <c r="L172" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
     <row r="173" spans="2:20" x14ac:dyDescent="0.25">
@@ -7408,13 +7426,13 @@
         <v>109</v>
       </c>
       <c r="H173" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="I173" t="s">
         <v>415</v>
       </c>
       <c r="L173" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
     </row>
     <row r="174" spans="2:20" x14ac:dyDescent="0.25">
@@ -7434,13 +7452,13 @@
         <v>109</v>
       </c>
       <c r="H174" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="I174" t="s">
         <v>415</v>
       </c>
       <c r="L174" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
     </row>
     <row r="175" spans="2:20" x14ac:dyDescent="0.25">
@@ -7460,16 +7478,16 @@
         <v>109</v>
       </c>
       <c r="H175" t="s">
-        <v>594</v>
+        <v>611</v>
       </c>
       <c r="I175" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="L175" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T175" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
     </row>
     <row r="176" spans="2:20" x14ac:dyDescent="0.25">
@@ -7489,16 +7507,16 @@
         <v>109</v>
       </c>
       <c r="H176" t="s">
-        <v>594</v>
+        <v>611</v>
       </c>
       <c r="I176" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="L176" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T176" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="177" spans="2:20" x14ac:dyDescent="0.25">
@@ -7518,16 +7536,16 @@
         <v>109</v>
       </c>
       <c r="H177" t="s">
-        <v>594</v>
+        <v>611</v>
       </c>
       <c r="I177" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="L177" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T177" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="178" spans="2:20" x14ac:dyDescent="0.25">
@@ -7547,16 +7565,16 @@
         <v>109</v>
       </c>
       <c r="H178" t="s">
-        <v>594</v>
+        <v>611</v>
       </c>
       <c r="I178" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="L178" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T178" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="179" spans="2:20" x14ac:dyDescent="0.25">
@@ -7576,13 +7594,13 @@
         <v>109</v>
       </c>
       <c r="H179" t="s">
-        <v>594</v>
+        <v>610</v>
       </c>
       <c r="I179" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="L179" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T179" t="s">
         <v>422</v>
@@ -7605,13 +7623,13 @@
         <v>109</v>
       </c>
       <c r="H180" t="s">
-        <v>594</v>
+        <v>611</v>
       </c>
       <c r="I180" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="L180" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="T180" t="s">
         <v>422</v>
@@ -7634,13 +7652,13 @@
         <v>115</v>
       </c>
       <c r="H181" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="I181" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="T181" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="182" spans="2:20" x14ac:dyDescent="0.25">
@@ -7660,13 +7678,13 @@
         <v>115</v>
       </c>
       <c r="H182" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="I182" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="T182" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="183" spans="2:20" x14ac:dyDescent="0.25">
@@ -7686,13 +7704,13 @@
         <v>115</v>
       </c>
       <c r="H183" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="I183" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="T183" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="184" spans="2:20" x14ac:dyDescent="0.25">
@@ -7712,10 +7730,10 @@
         <v>116</v>
       </c>
       <c r="H184" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="I184" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J184">
         <v>6</v>
@@ -7741,7 +7759,7 @@
         <v>116</v>
       </c>
       <c r="H185" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="I185" t="s">
         <v>424</v>
@@ -7767,10 +7785,10 @@
         <v>117</v>
       </c>
       <c r="H186" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="I186" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="187" spans="2:20" x14ac:dyDescent="0.25">
@@ -7790,10 +7808,10 @@
         <v>117</v>
       </c>
       <c r="H187" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="I187" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
     </row>
     <row r="188" spans="2:20" x14ac:dyDescent="0.25">
@@ -7816,7 +7834,7 @@
         <v>134</v>
       </c>
       <c r="H188" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="I188" t="s">
         <v>415</v>
@@ -7839,13 +7857,13 @@
         <v>135</v>
       </c>
       <c r="H189" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="I189" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="T189" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="190" spans="2:20" x14ac:dyDescent="0.25">
@@ -7865,13 +7883,13 @@
         <v>135</v>
       </c>
       <c r="H190" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="I190" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="T190" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="191" spans="2:20" x14ac:dyDescent="0.25">
@@ -7891,13 +7909,13 @@
         <v>135</v>
       </c>
       <c r="H191" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="I191" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
       <c r="T191" t="s">
-        <v>604</v>
+        <v>454</v>
       </c>
     </row>
     <row r="192" spans="2:20" x14ac:dyDescent="0.25">
@@ -7917,13 +7935,13 @@
         <v>135</v>
       </c>
       <c r="H192" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="I192" t="s">
         <v>424</v>
       </c>
       <c r="T192" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="193" spans="2:20" x14ac:dyDescent="0.25">
@@ -7943,13 +7961,13 @@
         <v>135</v>
       </c>
       <c r="H193" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="I193" t="s">
         <v>424</v>
       </c>
       <c r="T193" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="194" spans="2:20" x14ac:dyDescent="0.25">
@@ -7969,13 +7987,13 @@
         <v>135</v>
       </c>
       <c r="H194" t="s">
-        <v>605</v>
+        <v>596</v>
       </c>
       <c r="I194" t="s">
         <v>424</v>
       </c>
       <c r="T194" t="s">
-        <v>604</v>
+        <v>454</v>
       </c>
     </row>
     <row r="195" spans="2:20" x14ac:dyDescent="0.25">
@@ -7995,13 +8013,13 @@
         <v>151</v>
       </c>
       <c r="H195" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="I195" t="s">
         <v>424</v>
       </c>
       <c r="M195" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="196" spans="2:20" x14ac:dyDescent="0.25">
@@ -8021,13 +8039,13 @@
         <v>151</v>
       </c>
       <c r="H196" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="I196" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="M196" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
     </row>
     <row r="197" spans="2:20" x14ac:dyDescent="0.25">
@@ -8047,13 +8065,13 @@
         <v>151</v>
       </c>
       <c r="H197" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="I197" t="s">
         <v>424</v>
       </c>
       <c r="M197" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
     </row>
     <row r="198" spans="2:20" x14ac:dyDescent="0.25">
@@ -8073,13 +8091,13 @@
         <v>151</v>
       </c>
       <c r="H198" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="I198" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="M198" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
     </row>
     <row r="199" spans="2:20" x14ac:dyDescent="0.25">
@@ -8099,13 +8117,13 @@
         <v>151</v>
       </c>
       <c r="H199" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="I199" t="s">
         <v>424</v>
       </c>
       <c r="M199" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="200" spans="2:20" x14ac:dyDescent="0.25">
@@ -8125,13 +8143,13 @@
         <v>151</v>
       </c>
       <c r="H200" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="I200" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="M200" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
     </row>
     <row r="201" spans="2:20" x14ac:dyDescent="0.25">
@@ -8151,13 +8169,13 @@
         <v>151</v>
       </c>
       <c r="H201" t="s">
-        <v>606</v>
+        <v>597</v>
       </c>
       <c r="I201" t="s">
         <v>424</v>
       </c>
       <c r="M201" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="202" spans="2:20" x14ac:dyDescent="0.25">
@@ -8177,13 +8195,13 @@
         <v>151</v>
       </c>
       <c r="H202" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="I202" t="s">
-        <v>607</v>
+        <v>598</v>
       </c>
       <c r="M202" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
     </row>
     <row r="203" spans="2:20" x14ac:dyDescent="0.25">
@@ -8203,10 +8221,10 @@
         <v>152</v>
       </c>
       <c r="H203" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="I203" t="s">
-        <v>610</v>
+        <v>601</v>
       </c>
       <c r="J203">
         <v>3</v>
@@ -8232,11 +8250,11 @@
         <v>609</v>
       </c>
       <c r="I204" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U204"/>
+  <autoFilter ref="A1:U204" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState ref="B2:T204">
     <sortCondition ref="G2:G204"/>
     <sortCondition ref="E2:E204"/>

</xml_diff>

<commit_message>
extract syb data for new series following draft dsd
</commit_message>
<xml_diff>
--- a/unsd/UNSYB/data/SYB series mapping to DSD.xlsx
+++ b/unsd/UNSYB/data/SYB series mapping to DSD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\unsd\UNSYB\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47465C14-E75E-4336-9394-1D04C6CE6A0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89700B03-AB0B-4E91-8CD7-D11DFD9D95DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -796,9 +796,6 @@
     <t>int%</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentage of individuals using the internet 											</t>
-  </si>
-  <si>
     <t>dentnum</t>
   </si>
   <si>
@@ -1889,6 +1886,9 @@
   </si>
   <si>
     <t>Total traffic - distance</t>
+  </si>
+  <si>
+    <t>Percentage of individuals using the internet</t>
   </si>
 </sst>
 </file>
@@ -2746,10 +2746,10 @@
   <dimension ref="A1:T204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F149" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H58" sqref="H58"/>
+      <selection pane="bottomRight" activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,7 +2765,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2786,54 +2786,54 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
+        <v>412</v>
+      </c>
+      <c r="I1" t="s">
         <v>413</v>
       </c>
-      <c r="I1" t="s">
-        <v>414</v>
-      </c>
       <c r="J1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="K1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="L1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="M1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="N1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="O1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="P1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Q1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="R1" t="s">
+        <v>415</v>
+      </c>
+      <c r="S1" t="s">
+        <v>439</v>
+      </c>
+      <c r="T1" t="s">
         <v>416</v>
-      </c>
-      <c r="S1" t="s">
-        <v>440</v>
-      </c>
-      <c r="T1" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D2">
         <v>1641</v>
       </c>
       <c r="E2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F2">
         <v>24</v>
@@ -2842,27 +2842,27 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I2" t="s">
+        <v>450</v>
+      </c>
+      <c r="S2" t="s">
+        <v>457</v>
+      </c>
+      <c r="T2" t="s">
         <v>451</v>
-      </c>
-      <c r="S2" t="s">
-        <v>458</v>
-      </c>
-      <c r="T2" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D3">
         <v>1629</v>
       </c>
       <c r="E3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F3">
         <v>24</v>
@@ -2871,27 +2871,27 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I3" t="s">
+        <v>450</v>
+      </c>
+      <c r="S3" t="s">
+        <v>458</v>
+      </c>
+      <c r="T3" t="s">
         <v>451</v>
-      </c>
-      <c r="S3" t="s">
-        <v>459</v>
-      </c>
-      <c r="T3" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D4">
         <v>1642</v>
       </c>
       <c r="E4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F4">
         <v>24</v>
@@ -2900,27 +2900,27 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="T4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D5">
         <v>1630</v>
       </c>
       <c r="E5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F5">
         <v>24</v>
@@ -2929,27 +2929,27 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="T5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D6">
         <v>1643</v>
       </c>
       <c r="E6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F6">
         <v>24</v>
@@ -2958,27 +2958,27 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="T6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D7">
         <v>1631</v>
       </c>
       <c r="E7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F7">
         <v>24</v>
@@ -2987,16 +2987,16 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="S7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="T7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -3016,19 +3016,19 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J8">
         <v>3</v>
       </c>
       <c r="S8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -3048,19 +3048,19 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J9">
         <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -3080,19 +3080,19 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J10">
         <v>3</v>
       </c>
       <c r="S10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="T10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -3112,13 +3112,13 @@
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I11" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O11" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -3138,13 +3138,13 @@
         <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O12" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -3164,13 +3164,13 @@
         <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O13" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -3190,13 +3190,13 @@
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I14" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="O14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -3216,10 +3216,10 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I15" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -3239,10 +3239,10 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I16" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
@@ -3262,10 +3262,10 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I17" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
@@ -3285,10 +3285,10 @@
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I18" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
@@ -3308,10 +3308,10 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I19" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
@@ -3331,10 +3331,10 @@
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
@@ -3354,10 +3354,10 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
@@ -3377,13 +3377,13 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I22" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="S22" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
@@ -3403,13 +3403,13 @@
         <v>8</v>
       </c>
       <c r="H23" t="s">
+        <v>437</v>
+      </c>
+      <c r="I23" t="s">
         <v>438</v>
       </c>
-      <c r="I23" t="s">
-        <v>439</v>
-      </c>
       <c r="S23" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -3429,13 +3429,13 @@
         <v>8</v>
       </c>
       <c r="H24" t="s">
+        <v>437</v>
+      </c>
+      <c r="I24" t="s">
         <v>438</v>
       </c>
-      <c r="I24" t="s">
-        <v>439</v>
-      </c>
       <c r="S24" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -3455,13 +3455,13 @@
         <v>8</v>
       </c>
       <c r="H25" t="s">
+        <v>437</v>
+      </c>
+      <c r="I25" t="s">
         <v>438</v>
       </c>
-      <c r="I25" t="s">
-        <v>439</v>
-      </c>
       <c r="S25" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -3481,10 +3481,10 @@
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I26" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -3504,10 +3504,10 @@
         <v>8</v>
       </c>
       <c r="H27" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I27" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
@@ -3527,10 +3527,10 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
@@ -3556,7 +3556,7 @@
         <v>23</v>
       </c>
       <c r="I29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.25">
@@ -3582,7 +3582,7 @@
         <v>31</v>
       </c>
       <c r="I30" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.25">
@@ -3608,7 +3608,7 @@
         <v>25</v>
       </c>
       <c r="I31" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
@@ -3634,7 +3634,7 @@
         <v>35</v>
       </c>
       <c r="I32" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -3660,7 +3660,7 @@
         <v>29</v>
       </c>
       <c r="I33" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -3686,21 +3686,21 @@
         <v>37</v>
       </c>
       <c r="I34" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D35" s="1">
         <v>1581</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F35" s="1">
         <v>37</v>
@@ -3709,27 +3709,27 @@
         <v>18</v>
       </c>
       <c r="H35" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="I35" s="1" t="s">
-        <v>480</v>
-      </c>
       <c r="N35" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D36" s="1">
         <v>1582</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F36" s="1">
         <v>37</v>
@@ -3738,27 +3738,27 @@
         <v>18</v>
       </c>
       <c r="H36" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="I36" s="1" t="s">
-        <v>480</v>
-      </c>
       <c r="N36" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D37" s="1">
         <v>1583</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F37" s="1">
         <v>37</v>
@@ -3767,13 +3767,13 @@
         <v>18</v>
       </c>
       <c r="H37" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>479</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>480</v>
-      </c>
       <c r="N37" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -3793,10 +3793,10 @@
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I38" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J38">
         <v>6</v>
@@ -3822,10 +3822,10 @@
         <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I39" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J39">
         <v>6</v>
@@ -3848,10 +3848,10 @@
         <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I40" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
@@ -3871,10 +3871,10 @@
         <v>19</v>
       </c>
       <c r="H41" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I41" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -3894,16 +3894,16 @@
         <v>23</v>
       </c>
       <c r="H42" t="s">
+        <v>485</v>
+      </c>
+      <c r="I42" t="s">
+        <v>427</v>
+      </c>
+      <c r="K42" t="s">
+        <v>487</v>
+      </c>
+      <c r="N42" t="s">
         <v>486</v>
-      </c>
-      <c r="I42" t="s">
-        <v>428</v>
-      </c>
-      <c r="K42" t="s">
-        <v>488</v>
-      </c>
-      <c r="N42" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -3923,16 +3923,16 @@
         <v>23</v>
       </c>
       <c r="H43" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I43" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K43" t="s">
+        <v>487</v>
+      </c>
+      <c r="N43" t="s">
         <v>488</v>
-      </c>
-      <c r="N43" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -3952,16 +3952,16 @@
         <v>23</v>
       </c>
       <c r="H44" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K44" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N44" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3981,16 +3981,16 @@
         <v>23</v>
       </c>
       <c r="H45" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I45" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K45" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N45" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -4010,27 +4010,27 @@
         <v>23</v>
       </c>
       <c r="H46" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I46" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K46" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N46" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D47">
         <v>1579</v>
       </c>
       <c r="E47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F47">
         <v>74</v>
@@ -4039,16 +4039,16 @@
         <v>23</v>
       </c>
       <c r="H47" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I47" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K47" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N47" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -4068,16 +4068,16 @@
         <v>23</v>
       </c>
       <c r="H48" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I48" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K48" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N48" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
@@ -4097,16 +4097,16 @@
         <v>23</v>
       </c>
       <c r="H49" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I49" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K49" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N49" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.25">
@@ -4126,16 +4126,16 @@
         <v>23</v>
       </c>
       <c r="H50" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I50" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K50" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N50" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
@@ -4155,16 +4155,16 @@
         <v>23</v>
       </c>
       <c r="H51" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I51" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K51" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N51" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
@@ -4184,27 +4184,27 @@
         <v>23</v>
       </c>
       <c r="H52" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I52" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K52" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N52" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D53">
         <v>1580</v>
       </c>
       <c r="E53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F53">
         <v>74</v>
@@ -4213,16 +4213,16 @@
         <v>23</v>
       </c>
       <c r="H53" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I53" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K53" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N53" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.25">
@@ -4242,16 +4242,16 @@
         <v>23</v>
       </c>
       <c r="H54" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I54" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K54" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N54" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.25">
@@ -4271,27 +4271,27 @@
         <v>23</v>
       </c>
       <c r="H55" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I55" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K55" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N55" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D56">
         <v>1567</v>
       </c>
       <c r="E56" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F56">
         <v>74</v>
@@ -4300,16 +4300,16 @@
         <v>23</v>
       </c>
       <c r="H56" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I56" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K56" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N56" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
@@ -4329,13 +4329,13 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I57" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K57" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.25">
@@ -4355,24 +4355,24 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I58" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K58" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D59">
         <v>1586</v>
       </c>
       <c r="E59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F59">
         <v>85</v>
@@ -4381,27 +4381,27 @@
         <v>49</v>
       </c>
       <c r="H59" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I59" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N59" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="S59" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D60">
         <v>1585</v>
       </c>
       <c r="E60" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F60">
         <v>85</v>
@@ -4410,27 +4410,27 @@
         <v>49</v>
       </c>
       <c r="H60" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I60" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N60" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="S60" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D61">
         <v>1584</v>
       </c>
       <c r="E61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F61">
         <v>85</v>
@@ -4439,27 +4439,27 @@
         <v>49</v>
       </c>
       <c r="H61" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I61" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N61" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="S61" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="62" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D62">
         <v>1589</v>
       </c>
       <c r="E62" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F62">
         <v>85</v>
@@ -4468,27 +4468,27 @@
         <v>49</v>
       </c>
       <c r="H62" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I62" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N62" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S62" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D63">
         <v>1588</v>
       </c>
       <c r="E63" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F63">
         <v>85</v>
@@ -4497,27 +4497,27 @@
         <v>49</v>
       </c>
       <c r="H63" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I63" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N63" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S63" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="64" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D64">
         <v>1587</v>
       </c>
       <c r="E64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F64">
         <v>85</v>
@@ -4526,27 +4526,27 @@
         <v>49</v>
       </c>
       <c r="H64" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I64" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N64" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="S64" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="65" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D65">
         <v>1592</v>
       </c>
       <c r="E65" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F65">
         <v>85</v>
@@ -4555,27 +4555,27 @@
         <v>49</v>
       </c>
       <c r="H65" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I65" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N65" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="S65" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="66" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D66">
         <v>1591</v>
       </c>
       <c r="E66" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F66">
         <v>85</v>
@@ -4584,27 +4584,27 @@
         <v>49</v>
       </c>
       <c r="H66" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I66" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N66" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="S66" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D67">
         <v>1590</v>
       </c>
       <c r="E67" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F67">
         <v>85</v>
@@ -4613,16 +4613,16 @@
         <v>49</v>
       </c>
       <c r="H67" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I67" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N67" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="S67" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
@@ -4642,10 +4642,10 @@
         <v>57</v>
       </c>
       <c r="H68" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I68" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J68">
         <v>6</v>
@@ -4668,10 +4668,10 @@
         <v>57</v>
       </c>
       <c r="H69" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I69" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J69">
         <v>6</v>
@@ -4694,10 +4694,10 @@
         <v>58</v>
       </c>
       <c r="H70" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="I70" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J70">
         <v>3</v>
@@ -4720,10 +4720,10 @@
         <v>58</v>
       </c>
       <c r="H71" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="I71" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="J71">
         <v>3</v>
@@ -4746,10 +4746,10 @@
         <v>60</v>
       </c>
       <c r="H72" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="I72" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J72">
         <v>3</v>
@@ -4772,10 +4772,10 @@
         <v>60</v>
       </c>
       <c r="H73" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="I73" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="J73">
         <v>3</v>
@@ -4798,10 +4798,10 @@
         <v>61</v>
       </c>
       <c r="H74" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I74" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J74">
         <v>6</v>
@@ -4824,10 +4824,10 @@
         <v>61</v>
       </c>
       <c r="H75" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I75" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J75">
         <v>6</v>
@@ -4850,10 +4850,10 @@
         <v>61</v>
       </c>
       <c r="H76" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="I76" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J76">
         <v>3</v>
@@ -4876,10 +4876,10 @@
         <v>61</v>
       </c>
       <c r="H77" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="I77" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="J77">
         <v>6</v>
@@ -4902,10 +4902,10 @@
         <v>61</v>
       </c>
       <c r="H78" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I78" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J78">
         <v>6</v>
@@ -4928,10 +4928,10 @@
         <v>61</v>
       </c>
       <c r="H79" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I79" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J79">
         <v>6</v>
@@ -4954,10 +4954,10 @@
         <v>61</v>
       </c>
       <c r="H80" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I80" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="J80">
         <v>3</v>
@@ -4980,10 +4980,10 @@
         <v>61</v>
       </c>
       <c r="H81" t="s">
+        <v>504</v>
+      </c>
+      <c r="I81" t="s">
         <v>505</v>
-      </c>
-      <c r="I81" t="s">
-        <v>506</v>
       </c>
       <c r="J81">
         <v>6</v>
@@ -4991,13 +4991,13 @@
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D82">
         <v>1576</v>
       </c>
       <c r="E82" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F82">
         <v>78</v>
@@ -5006,10 +5006,10 @@
         <v>64</v>
       </c>
       <c r="H82" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I82" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.25">
@@ -5029,10 +5029,10 @@
         <v>64</v>
       </c>
       <c r="H83" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I83" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J83">
         <v>3</v>
@@ -5040,13 +5040,13 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D84">
         <v>1578</v>
       </c>
       <c r="E84" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F84">
         <v>78</v>
@@ -5055,10 +5055,10 @@
         <v>64</v>
       </c>
       <c r="H84" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I84" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.25">
@@ -5078,10 +5078,10 @@
         <v>64</v>
       </c>
       <c r="H85" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I85" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J85">
         <v>3</v>
@@ -5104,15 +5104,15 @@
         <v>64</v>
       </c>
       <c r="H86" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I86" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="87" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>204</v>
@@ -5130,10 +5130,10 @@
         <v>64</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J87" s="1">
         <v>3</v>
@@ -5141,13 +5141,13 @@
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D88">
         <v>1577</v>
       </c>
       <c r="E88" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F88">
         <v>78</v>
@@ -5156,10 +5156,10 @@
         <v>64</v>
       </c>
       <c r="H88" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I88" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.25">
@@ -5179,10 +5179,10 @@
         <v>64</v>
       </c>
       <c r="H89" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I89" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="J89">
         <v>3</v>
@@ -5190,13 +5190,13 @@
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D90">
         <v>1595</v>
       </c>
       <c r="E90" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F90">
         <v>29</v>
@@ -5205,21 +5205,21 @@
         <v>65</v>
       </c>
       <c r="H90" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I90" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D91">
         <v>1594</v>
       </c>
       <c r="E91" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F91">
         <v>29</v>
@@ -5228,21 +5228,21 @@
         <v>65</v>
       </c>
       <c r="H91" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="I91" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D92">
         <v>1593</v>
       </c>
       <c r="E92" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="F92">
         <v>29</v>
@@ -5251,21 +5251,21 @@
         <v>65</v>
       </c>
       <c r="H92" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="I92" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D93">
         <v>1597</v>
       </c>
       <c r="E93" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F93">
         <v>29</v>
@@ -5274,21 +5274,21 @@
         <v>65</v>
       </c>
       <c r="H93" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I93" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D94">
         <v>1596</v>
       </c>
       <c r="E94" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F94">
         <v>29</v>
@@ -5297,10 +5297,10 @@
         <v>65</v>
       </c>
       <c r="H94" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="I94" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -5320,16 +5320,16 @@
         <v>66</v>
       </c>
       <c r="H95" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I95" t="s">
+        <v>534</v>
+      </c>
+      <c r="M95" t="s">
         <v>535</v>
       </c>
-      <c r="M95" t="s">
-        <v>536</v>
-      </c>
       <c r="S95" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.25">
@@ -5349,16 +5349,16 @@
         <v>66</v>
       </c>
       <c r="H96" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I96" t="s">
+        <v>534</v>
+      </c>
+      <c r="M96" t="s">
         <v>535</v>
       </c>
-      <c r="M96" t="s">
-        <v>536</v>
-      </c>
       <c r="S96" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
@@ -5378,16 +5378,16 @@
         <v>66</v>
       </c>
       <c r="H97" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I97" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M97" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="S97" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
@@ -5407,16 +5407,16 @@
         <v>66</v>
       </c>
       <c r="H98" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I98" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M98" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="S98" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
@@ -5436,16 +5436,16 @@
         <v>66</v>
       </c>
       <c r="H99" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I99" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M99" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S99" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.25">
@@ -5465,16 +5465,16 @@
         <v>66</v>
       </c>
       <c r="H100" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I100" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M100" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="S100" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
@@ -5494,16 +5494,16 @@
         <v>66</v>
       </c>
       <c r="H101" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="I101" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="M101" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="S101" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
@@ -5523,10 +5523,10 @@
         <v>67</v>
       </c>
       <c r="H102" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="I102" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.25">
@@ -5546,10 +5546,10 @@
         <v>67</v>
       </c>
       <c r="H103" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I103" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
@@ -5569,15 +5569,15 @@
         <v>67</v>
       </c>
       <c r="H104" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I104" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="105" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>202</v>
@@ -5598,10 +5598,10 @@
         <v>68</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J105" s="1">
         <v>6</v>
@@ -5609,7 +5609,7 @@
     </row>
     <row r="106" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>96</v>
@@ -5630,10 +5630,10 @@
         <v>68</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J106" s="1">
         <v>6</v>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="107" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>120</v>
@@ -5662,10 +5662,10 @@
         <v>68</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J107" s="1">
         <v>6</v>
@@ -5673,7 +5673,7 @@
     </row>
     <row r="108" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>216</v>
@@ -5691,10 +5691,10 @@
         <v>74</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J108" s="1">
         <v>6</v>
@@ -5702,7 +5702,7 @@
     </row>
     <row r="109" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>214</v>
@@ -5720,10 +5720,10 @@
         <v>74</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J109" s="1">
         <v>6</v>
@@ -5731,7 +5731,7 @@
     </row>
     <row r="110" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>32</v>
@@ -5749,10 +5749,10 @@
         <v>74</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J110" s="1">
         <v>6</v>
@@ -5760,7 +5760,7 @@
     </row>
     <row r="111" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>92</v>
@@ -5781,15 +5781,15 @@
         <v>75</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="112" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>94</v>
@@ -5810,10 +5810,10 @@
         <v>75</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
@@ -5833,16 +5833,16 @@
         <v>77</v>
       </c>
       <c r="H113" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I113" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J113">
         <v>6</v>
       </c>
       <c r="K113" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
@@ -5862,27 +5862,27 @@
         <v>77</v>
       </c>
       <c r="H114" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I114" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J114">
         <v>6</v>
       </c>
       <c r="K114" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D115">
         <v>1555</v>
       </c>
       <c r="E115" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F115">
         <v>22</v>
@@ -5891,13 +5891,13 @@
         <v>77</v>
       </c>
       <c r="H115" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I115" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K115" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="116" spans="1:19" x14ac:dyDescent="0.25">
@@ -5917,27 +5917,27 @@
         <v>77</v>
       </c>
       <c r="H116" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I116" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J116">
         <v>6</v>
       </c>
       <c r="K116" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="117" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D117">
         <v>1617</v>
       </c>
       <c r="E117" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F117">
         <v>90</v>
@@ -5946,24 +5946,24 @@
         <v>78</v>
       </c>
       <c r="H117" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I117" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="118" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D118" s="1">
         <v>1614</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F118" s="1">
         <v>89</v>
@@ -5972,27 +5972,27 @@
         <v>78</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="119" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D119" s="1">
         <v>1610</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F119" s="1">
         <v>89</v>
@@ -6001,27 +6001,27 @@
         <v>78</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="S119" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="120" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D120" s="1">
         <v>1616</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F120" s="1">
         <v>89</v>
@@ -6030,27 +6030,27 @@
         <v>78</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="121" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D121" s="1">
         <v>1615</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F121" s="1">
         <v>89</v>
@@ -6059,27 +6059,27 @@
         <v>78</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="122" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D122" s="1">
         <v>1618</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F122" s="1">
         <v>90</v>
@@ -6088,24 +6088,24 @@
         <v>78</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="123" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D123" s="1">
         <v>1619</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F123" s="1">
         <v>90</v>
@@ -6114,24 +6114,24 @@
         <v>78</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="124" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D124" s="1">
         <v>1613</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F124" s="1">
         <v>90</v>
@@ -6140,15 +6140,15 @@
         <v>78</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="125" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>154</v>
@@ -6169,15 +6169,15 @@
         <v>83</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="126" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>156</v>
@@ -6198,15 +6198,15 @@
         <v>83</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="127" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>152</v>
@@ -6227,10 +6227,10 @@
         <v>83</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J127" s="1">
         <v>3</v>
@@ -6238,7 +6238,7 @@
     </row>
     <row r="128" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>172</v>
@@ -6256,18 +6256,18 @@
         <v>83</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q128" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="129" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>174</v>
@@ -6285,18 +6285,18 @@
         <v>83</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q129" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="130" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>170</v>
@@ -6314,13 +6314,13 @@
         <v>83</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="Q130" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="131" spans="1:18" x14ac:dyDescent="0.25">
@@ -6340,13 +6340,13 @@
         <v>84</v>
       </c>
       <c r="H131" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I131" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q131" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="132" spans="1:18" x14ac:dyDescent="0.25">
@@ -6366,13 +6366,13 @@
         <v>84</v>
       </c>
       <c r="H132" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I132" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q132" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="133" spans="1:18" x14ac:dyDescent="0.25">
@@ -6392,13 +6392,13 @@
         <v>84</v>
       </c>
       <c r="H133" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="I133" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q133" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="134" spans="1:18" x14ac:dyDescent="0.25">
@@ -6418,13 +6418,13 @@
         <v>84</v>
       </c>
       <c r="H134" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I134" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q134" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="135" spans="1:18" x14ac:dyDescent="0.25">
@@ -6444,13 +6444,13 @@
         <v>84</v>
       </c>
       <c r="H135" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I135" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q135" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="136" spans="1:18" x14ac:dyDescent="0.25">
@@ -6470,13 +6470,13 @@
         <v>84</v>
       </c>
       <c r="H136" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I136" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q136" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="137" spans="1:18" x14ac:dyDescent="0.25">
@@ -6496,13 +6496,13 @@
         <v>84</v>
       </c>
       <c r="H137" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I137" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q137" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="138" spans="1:18" x14ac:dyDescent="0.25">
@@ -6522,13 +6522,13 @@
         <v>84</v>
       </c>
       <c r="H138" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I138" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q138" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="139" spans="1:18" x14ac:dyDescent="0.25">
@@ -6548,13 +6548,13 @@
         <v>84</v>
       </c>
       <c r="H139" t="s">
+        <v>418</v>
+      </c>
+      <c r="I139" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q139" t="s">
         <v>419</v>
-      </c>
-      <c r="I139" t="s">
-        <v>415</v>
-      </c>
-      <c r="Q139" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="140" spans="1:18" x14ac:dyDescent="0.25">
@@ -6574,13 +6574,13 @@
         <v>84</v>
       </c>
       <c r="H140" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I140" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q140" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="141" spans="1:18" x14ac:dyDescent="0.25">
@@ -6600,13 +6600,13 @@
         <v>84</v>
       </c>
       <c r="H141" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I141" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q141" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="142" spans="1:18" x14ac:dyDescent="0.25">
@@ -6626,18 +6626,18 @@
         <v>84</v>
       </c>
       <c r="H142" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I142" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q142" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="143" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>38</v>
@@ -6655,18 +6655,18 @@
         <v>89</v>
       </c>
       <c r="H143" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="I143" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="R143" s="1" t="s">
         <v>435</v>
-      </c>
-      <c r="I143" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="R143" s="1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="144" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>40</v>
@@ -6684,18 +6684,18 @@
         <v>89</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="R144" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="145" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>212</v>
@@ -6718,7 +6718,7 @@
     </row>
     <row r="146" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>208</v>
@@ -6736,21 +6736,21 @@
         <v>89</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J146" s="1">
         <v>6</v>
       </c>
       <c r="S146" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="147" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>88</v>
@@ -6768,21 +6768,21 @@
         <v>89</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J147" s="1">
         <v>6</v>
       </c>
       <c r="S147" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="148" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>90</v>
@@ -6800,21 +6800,21 @@
         <v>89</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J148" s="1">
         <v>6</v>
       </c>
       <c r="S148" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="149" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>42</v>
@@ -6835,12 +6835,12 @@
         <v>43</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="150" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>210</v>
@@ -6858,10 +6858,10 @@
         <v>89</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J150" s="1">
         <v>3</v>
@@ -6869,13 +6869,13 @@
     </row>
     <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D151">
         <v>1605</v>
       </c>
       <c r="E151" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F151">
         <v>85</v>
@@ -6884,24 +6884,24 @@
         <v>94</v>
       </c>
       <c r="H151" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I151" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S151" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D152">
         <v>1604</v>
       </c>
       <c r="E152" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F152">
         <v>85</v>
@@ -6910,24 +6910,24 @@
         <v>94</v>
       </c>
       <c r="H152" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I152" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S152" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D153">
         <v>1603</v>
       </c>
       <c r="E153" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F153">
         <v>85</v>
@@ -6936,24 +6936,24 @@
         <v>94</v>
       </c>
       <c r="H153" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I153" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S153" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D154">
         <v>1602</v>
       </c>
       <c r="E154" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F154">
         <v>85</v>
@@ -6962,24 +6962,24 @@
         <v>94</v>
       </c>
       <c r="H154" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I154" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S154" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D155">
         <v>1601</v>
       </c>
       <c r="E155" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F155">
         <v>85</v>
@@ -6988,24 +6988,24 @@
         <v>94</v>
       </c>
       <c r="H155" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I155" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S155" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D156">
         <v>1600</v>
       </c>
       <c r="E156" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F156">
         <v>85</v>
@@ -7014,27 +7014,27 @@
         <v>94</v>
       </c>
       <c r="H156" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I156" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S156" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="157" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D157" s="1">
         <v>1606</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F157" s="1">
         <v>34</v>
@@ -7043,24 +7043,24 @@
         <v>98</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="158" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D158" s="1">
         <v>1607</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F158" s="1">
         <v>34</v>
@@ -7069,21 +7069,21 @@
         <v>98</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D159">
         <v>1608</v>
       </c>
       <c r="E159" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F159">
         <v>22</v>
@@ -7092,21 +7092,21 @@
         <v>103</v>
       </c>
       <c r="H159" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I159" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B160" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D160">
         <v>1609</v>
       </c>
       <c r="E160" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F160">
         <v>22</v>
@@ -7115,10 +7115,10 @@
         <v>103</v>
       </c>
       <c r="H160" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="I160" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J160">
         <v>6</v>
@@ -7126,13 +7126,13 @@
     </row>
     <row r="161" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D161">
         <v>1624</v>
       </c>
       <c r="E161" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F161">
         <v>92</v>
@@ -7141,21 +7141,21 @@
         <v>104</v>
       </c>
       <c r="H161" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I161" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="162" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D162">
         <v>1621</v>
       </c>
       <c r="E162" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F162">
         <v>92</v>
@@ -7164,21 +7164,21 @@
         <v>104</v>
       </c>
       <c r="H162" t="s">
+        <v>574</v>
+      </c>
+      <c r="I162" t="s">
         <v>575</v>
-      </c>
-      <c r="I162" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="163" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D163">
         <v>1625</v>
       </c>
       <c r="E163" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F163">
         <v>92</v>
@@ -7187,21 +7187,21 @@
         <v>104</v>
       </c>
       <c r="H163" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I163" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="164" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D164">
         <v>1622</v>
       </c>
       <c r="E164" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F164">
         <v>92</v>
@@ -7210,24 +7210,24 @@
         <v>104</v>
       </c>
       <c r="H164" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I164" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S164" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="165" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D165">
         <v>1623</v>
       </c>
       <c r="E165" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F165">
         <v>92</v>
@@ -7236,24 +7236,24 @@
         <v>104</v>
       </c>
       <c r="H165" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I165" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="S165" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="166" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D166">
         <v>1628</v>
       </c>
       <c r="E166" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F166">
         <v>92</v>
@@ -7262,21 +7262,21 @@
         <v>104</v>
       </c>
       <c r="H166" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I166" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="167" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D167">
         <v>1627</v>
       </c>
       <c r="E167" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F167">
         <v>92</v>
@@ -7285,21 +7285,21 @@
         <v>104</v>
       </c>
       <c r="H167" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I167" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="168" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B168" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D168">
         <v>1626</v>
       </c>
       <c r="E168" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F168">
         <v>92</v>
@@ -7308,10 +7308,10 @@
         <v>104</v>
       </c>
       <c r="H168" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="I168" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="169" spans="2:20" x14ac:dyDescent="0.25">
@@ -7322,7 +7322,7 @@
         <v>1491</v>
       </c>
       <c r="E169" t="s">
-        <v>257</v>
+        <v>621</v>
       </c>
       <c r="F169">
         <v>18</v>
@@ -7331,10 +7331,10 @@
         <v>106</v>
       </c>
       <c r="H169" t="s">
-        <v>257</v>
+        <v>621</v>
       </c>
       <c r="I169" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="170" spans="2:20" x14ac:dyDescent="0.25">
@@ -7354,10 +7354,10 @@
         <v>107</v>
       </c>
       <c r="H170" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I170" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="171" spans="2:20" x14ac:dyDescent="0.25">
@@ -7377,21 +7377,21 @@
         <v>107</v>
       </c>
       <c r="H171" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="I171" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="172" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D172">
         <v>1638</v>
       </c>
       <c r="E172" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F172">
         <v>24</v>
@@ -7400,24 +7400,24 @@
         <v>109</v>
       </c>
       <c r="H172" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I172" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L172" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="173" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D173">
         <v>1640</v>
       </c>
       <c r="E173" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F173">
         <v>24</v>
@@ -7426,24 +7426,24 @@
         <v>109</v>
       </c>
       <c r="H173" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I173" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L173" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="174" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B174" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D174">
         <v>1639</v>
       </c>
       <c r="E174" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F174">
         <v>24</v>
@@ -7452,24 +7452,24 @@
         <v>109</v>
       </c>
       <c r="H174" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I174" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="L174" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="175" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D175">
         <v>1634</v>
       </c>
       <c r="E175" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F175">
         <v>24</v>
@@ -7478,27 +7478,27 @@
         <v>109</v>
       </c>
       <c r="H175" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I175" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L175" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T175" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="176" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B176" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D176">
         <v>1635</v>
       </c>
       <c r="E176" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F176">
         <v>24</v>
@@ -7507,27 +7507,27 @@
         <v>109</v>
       </c>
       <c r="H176" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I176" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L176" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T176" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="177" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D177">
         <v>1636</v>
       </c>
       <c r="E177" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F177">
         <v>24</v>
@@ -7536,27 +7536,27 @@
         <v>109</v>
       </c>
       <c r="H177" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I177" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L177" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T177" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="178" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B178" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D178">
         <v>1637</v>
       </c>
       <c r="E178" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F178">
         <v>24</v>
@@ -7565,27 +7565,27 @@
         <v>109</v>
       </c>
       <c r="H178" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I178" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L178" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T178" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="179" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D179">
         <v>1632</v>
       </c>
       <c r="E179" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F179">
         <v>24</v>
@@ -7594,27 +7594,27 @@
         <v>109</v>
       </c>
       <c r="H179" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I179" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L179" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T179" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="180" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B180" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D180">
         <v>1633</v>
       </c>
       <c r="E180" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F180">
         <v>24</v>
@@ -7623,16 +7623,16 @@
         <v>109</v>
       </c>
       <c r="H180" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I180" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L180" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="T180" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="181" spans="2:20" x14ac:dyDescent="0.25">
@@ -7652,13 +7652,13 @@
         <v>115</v>
       </c>
       <c r="H181" t="s">
+        <v>587</v>
+      </c>
+      <c r="I181" t="s">
         <v>588</v>
       </c>
-      <c r="I181" t="s">
-        <v>589</v>
-      </c>
       <c r="T181" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="182" spans="2:20" x14ac:dyDescent="0.25">
@@ -7678,13 +7678,13 @@
         <v>115</v>
       </c>
       <c r="H182" t="s">
+        <v>587</v>
+      </c>
+      <c r="I182" t="s">
         <v>588</v>
       </c>
-      <c r="I182" t="s">
-        <v>589</v>
-      </c>
       <c r="T182" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="183" spans="2:20" x14ac:dyDescent="0.25">
@@ -7704,13 +7704,13 @@
         <v>115</v>
       </c>
       <c r="H183" t="s">
+        <v>587</v>
+      </c>
+      <c r="I183" t="s">
         <v>588</v>
       </c>
-      <c r="I183" t="s">
-        <v>589</v>
-      </c>
       <c r="T183" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="184" spans="2:20" x14ac:dyDescent="0.25">
@@ -7730,10 +7730,10 @@
         <v>116</v>
       </c>
       <c r="H184" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="I184" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J184">
         <v>6</v>
@@ -7759,10 +7759,10 @@
         <v>116</v>
       </c>
       <c r="H185" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="I185" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J185">
         <v>3</v>
@@ -7770,13 +7770,13 @@
     </row>
     <row r="186" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D186">
         <v>1572</v>
       </c>
       <c r="E186" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F186">
         <v>91</v>
@@ -7785,21 +7785,21 @@
         <v>117</v>
       </c>
       <c r="H186" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="I186" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="187" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D187">
         <v>1573</v>
       </c>
       <c r="E187" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F187">
         <v>91</v>
@@ -7808,10 +7808,10 @@
         <v>117</v>
       </c>
       <c r="H187" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I187" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="188" spans="2:20" x14ac:dyDescent="0.25">
@@ -7834,10 +7834,10 @@
         <v>134</v>
       </c>
       <c r="H188" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="I188" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="189" spans="2:20" x14ac:dyDescent="0.25">
@@ -7857,13 +7857,13 @@
         <v>135</v>
       </c>
       <c r="H189" t="s">
+        <v>593</v>
+      </c>
+      <c r="I189" t="s">
         <v>594</v>
       </c>
-      <c r="I189" t="s">
-        <v>595</v>
-      </c>
       <c r="T189" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="190" spans="2:20" x14ac:dyDescent="0.25">
@@ -7883,13 +7883,13 @@
         <v>135</v>
       </c>
       <c r="H190" t="s">
+        <v>593</v>
+      </c>
+      <c r="I190" t="s">
         <v>594</v>
       </c>
-      <c r="I190" t="s">
-        <v>595</v>
-      </c>
       <c r="T190" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="191" spans="2:20" x14ac:dyDescent="0.25">
@@ -7909,13 +7909,13 @@
         <v>135</v>
       </c>
       <c r="H191" t="s">
+        <v>593</v>
+      </c>
+      <c r="I191" t="s">
         <v>594</v>
       </c>
-      <c r="I191" t="s">
-        <v>595</v>
-      </c>
       <c r="T191" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="192" spans="2:20" x14ac:dyDescent="0.25">
@@ -7935,13 +7935,13 @@
         <v>135</v>
       </c>
       <c r="H192" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I192" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T192" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="193" spans="2:20" x14ac:dyDescent="0.25">
@@ -7961,13 +7961,13 @@
         <v>135</v>
       </c>
       <c r="H193" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I193" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T193" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="194" spans="2:20" x14ac:dyDescent="0.25">
@@ -7987,24 +7987,24 @@
         <v>135</v>
       </c>
       <c r="H194" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="I194" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="T194" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="195" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D195">
         <v>1511</v>
       </c>
       <c r="E195" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F195">
         <v>84</v>
@@ -8013,24 +8013,24 @@
         <v>151</v>
       </c>
       <c r="H195" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I195" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M195" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="196" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D196">
         <v>1512</v>
       </c>
       <c r="E196" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F196">
         <v>84</v>
@@ -8039,24 +8039,24 @@
         <v>151</v>
       </c>
       <c r="H196" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I196" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M196" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="197" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D197">
         <v>1513</v>
       </c>
       <c r="E197" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F197">
         <v>84</v>
@@ -8065,24 +8065,24 @@
         <v>151</v>
       </c>
       <c r="H197" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I197" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M197" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="198" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D198">
         <v>1516</v>
       </c>
       <c r="E198" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F198">
         <v>84</v>
@@ -8091,24 +8091,24 @@
         <v>151</v>
       </c>
       <c r="H198" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I198" t="s">
+        <v>597</v>
+      </c>
+      <c r="M198" t="s">
         <v>598</v>
-      </c>
-      <c r="M198" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="199" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D199">
         <v>1515</v>
       </c>
       <c r="E199" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F199">
         <v>84</v>
@@ -8117,24 +8117,24 @@
         <v>151</v>
       </c>
       <c r="H199" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I199" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M199" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="200" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D200">
         <v>1514</v>
       </c>
       <c r="E200" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F200">
         <v>84</v>
@@ -8143,24 +8143,24 @@
         <v>151</v>
       </c>
       <c r="H200" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I200" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M200" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="201" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D201">
         <v>1517</v>
       </c>
       <c r="E201" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F201">
         <v>84</v>
@@ -8169,24 +8169,24 @@
         <v>151</v>
       </c>
       <c r="H201" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I201" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="M201" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="202" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B202" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D202">
         <v>1519</v>
       </c>
       <c r="E202" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F202">
         <v>84</v>
@@ -8195,24 +8195,24 @@
         <v>151</v>
       </c>
       <c r="H202" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I202" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="M202" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="203" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D203">
         <v>1521</v>
       </c>
       <c r="E203" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F203">
         <v>3</v>
@@ -8221,10 +8221,10 @@
         <v>152</v>
       </c>
       <c r="H203" t="s">
+        <v>599</v>
+      </c>
+      <c r="I203" t="s">
         <v>600</v>
-      </c>
-      <c r="I203" t="s">
-        <v>601</v>
       </c>
       <c r="J203">
         <v>3</v>
@@ -8232,13 +8232,13 @@
     </row>
     <row r="204" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B204" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D204">
         <v>1520</v>
       </c>
       <c r="E204" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F204">
         <v>3</v>
@@ -8247,10 +8247,10 @@
         <v>152</v>
       </c>
       <c r="H204" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I204" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix typos and move to output folder
</commit_message>
<xml_diff>
--- a/unsd/UNSYB/data/SYB series mapping to DSD.xlsx
+++ b/unsd/UNSYB/data/SYB series mapping to DSD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L.GonzalezMorales\Documents\GitHub\FIS4SDGs\unsd\UNSYB\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89700B03-AB0B-4E91-8CD7-D11DFD9D95DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABDD85B-ECEE-47FD-B6BE-F2C0BD50E0DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="625">
   <si>
     <t>seriesCode</t>
   </si>
@@ -1387,9 +1387,6 @@
     <t>Tertiary</t>
   </si>
   <si>
-    <t>Gross enrollment ratio</t>
-  </si>
-  <si>
     <t>Invertebrates</t>
   </si>
   <si>
@@ -1402,9 +1399,6 @@
     <t>FEMALE</t>
   </si>
   <si>
-    <t>Number of students enrolled</t>
-  </si>
-  <si>
     <t>Threatened species</t>
   </si>
   <si>
@@ -1669,9 +1663,6 @@
     <t>Capital city population</t>
   </si>
   <si>
-    <t>Urban population</t>
-  </si>
-  <si>
     <t>Population mid-year estimates</t>
   </si>
   <si>
@@ -1714,12 +1705,6 @@
     <t>Other population of concern to UNHCR</t>
   </si>
   <si>
-    <t>Percentage of total population</t>
-  </si>
-  <si>
-    <t>Percentage of total urban population</t>
-  </si>
-  <si>
     <t>Population growth rate per annum</t>
   </si>
   <si>
@@ -1889,6 +1874,30 @@
   </si>
   <si>
     <t>Percentage of individuals using the internet</t>
+  </si>
+  <si>
+    <t>Capital city population as percent of total population</t>
+  </si>
+  <si>
+    <t>Percent of total urban population</t>
+  </si>
+  <si>
+    <t>Capital city population as percent of total urban population</t>
+  </si>
+  <si>
+    <t>Urban population as percent of total populatoin</t>
+  </si>
+  <si>
+    <t>Number of species</t>
+  </si>
+  <si>
+    <t>Number of students enrolled in formal education</t>
+  </si>
+  <si>
+    <t>Number of students</t>
+  </si>
+  <si>
+    <t>Gross educatoin enrollment ratio</t>
   </si>
 </sst>
 </file>
@@ -2746,10 +2755,10 @@
   <dimension ref="A1:T204"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F149" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E170" sqref="E170"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,7 +2774,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2798,16 +2807,16 @@
         <v>424</v>
       </c>
       <c r="L1" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="M1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="N1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="O1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="P1" t="s">
         <v>447</v>
@@ -2842,13 +2851,13 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>454</v>
+        <v>624</v>
       </c>
       <c r="I2" t="s">
         <v>450</v>
       </c>
       <c r="S2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T2" t="s">
         <v>451</v>
@@ -2871,13 +2880,13 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>454</v>
+        <v>624</v>
       </c>
       <c r="I3" t="s">
         <v>450</v>
       </c>
       <c r="S3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="T3" t="s">
         <v>451</v>
@@ -2900,13 +2909,13 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>454</v>
+        <v>624</v>
       </c>
       <c r="I4" t="s">
         <v>450</v>
       </c>
       <c r="S4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="T4" t="s">
         <v>452</v>
@@ -2929,13 +2938,13 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>454</v>
+        <v>624</v>
       </c>
       <c r="I5" t="s">
         <v>450</v>
       </c>
       <c r="S5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T5" t="s">
         <v>452</v>
@@ -2958,13 +2967,13 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>454</v>
+        <v>624</v>
       </c>
       <c r="I6" t="s">
         <v>450</v>
       </c>
       <c r="S6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="T6" t="s">
         <v>453</v>
@@ -2987,13 +2996,13 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>454</v>
+        <v>624</v>
       </c>
       <c r="I7" t="s">
         <v>450</v>
       </c>
       <c r="S7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="T7" t="s">
         <v>453</v>
@@ -3016,10 +3025,10 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>459</v>
+        <v>622</v>
       </c>
       <c r="I8" t="s">
-        <v>423</v>
+        <v>623</v>
       </c>
       <c r="J8">
         <v>3</v>
@@ -3048,10 +3057,10 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>459</v>
+        <v>622</v>
       </c>
       <c r="I9" t="s">
-        <v>423</v>
+        <v>623</v>
       </c>
       <c r="J9">
         <v>3</v>
@@ -3080,10 +3089,10 @@
         <v>1</v>
       </c>
       <c r="H10" t="s">
-        <v>459</v>
+        <v>622</v>
       </c>
       <c r="I10" t="s">
-        <v>423</v>
+        <v>623</v>
       </c>
       <c r="J10">
         <v>3</v>
@@ -3112,13 +3121,13 @@
         <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I11" t="s">
-        <v>423</v>
+        <v>621</v>
       </c>
       <c r="O11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -3138,13 +3147,13 @@
         <v>5</v>
       </c>
       <c r="H12" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I12" t="s">
-        <v>423</v>
+        <v>621</v>
       </c>
       <c r="O12" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -3164,10 +3173,10 @@
         <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I13" t="s">
-        <v>423</v>
+        <v>621</v>
       </c>
       <c r="O13" t="s">
         <v>421</v>
@@ -3190,10 +3199,10 @@
         <v>5</v>
       </c>
       <c r="H14" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I14" t="s">
-        <v>423</v>
+        <v>621</v>
       </c>
       <c r="O14" t="s">
         <v>425</v>
@@ -3216,7 +3225,7 @@
         <v>6</v>
       </c>
       <c r="H15" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I15" t="s">
         <v>414</v>
@@ -3239,7 +3248,7 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I16" t="s">
         <v>414</v>
@@ -3262,7 +3271,7 @@
         <v>6</v>
       </c>
       <c r="H17" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I17" t="s">
         <v>414</v>
@@ -3285,7 +3294,7 @@
         <v>6</v>
       </c>
       <c r="H18" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I18" t="s">
         <v>414</v>
@@ -3308,7 +3317,7 @@
         <v>6</v>
       </c>
       <c r="H19" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="I19" t="s">
         <v>414</v>
@@ -3331,7 +3340,7 @@
         <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I20" t="s">
         <v>414</v>
@@ -3354,7 +3363,7 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I21" t="s">
         <v>414</v>
@@ -3377,10 +3386,10 @@
         <v>8</v>
       </c>
       <c r="H22" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I22" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S22" t="s">
         <v>440</v>
@@ -3435,7 +3444,7 @@
         <v>438</v>
       </c>
       <c r="S24" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.25">
@@ -3461,7 +3470,7 @@
         <v>438</v>
       </c>
       <c r="S25" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.25">
@@ -3481,10 +3490,10 @@
         <v>8</v>
       </c>
       <c r="H26" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I26" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.25">
@@ -3527,10 +3536,10 @@
         <v>8</v>
       </c>
       <c r="H28" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I28" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
@@ -3691,7 +3700,7 @@
     </row>
     <row r="35" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>295</v>
@@ -3709,18 +3718,18 @@
         <v>18</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>297</v>
@@ -3738,18 +3747,18 @@
         <v>18</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>299</v>
@@ -3767,13 +3776,13 @@
         <v>18</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -3793,7 +3802,7 @@
         <v>19</v>
       </c>
       <c r="H38" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I38" t="s">
         <v>432</v>
@@ -3822,7 +3831,7 @@
         <v>19</v>
       </c>
       <c r="H39" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I39" t="s">
         <v>432</v>
@@ -3848,7 +3857,7 @@
         <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I40" t="s">
         <v>432</v>
@@ -3871,7 +3880,7 @@
         <v>19</v>
       </c>
       <c r="H41" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I41" t="s">
         <v>414</v>
@@ -3894,16 +3903,16 @@
         <v>23</v>
       </c>
       <c r="H42" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I42" t="s">
         <v>427</v>
       </c>
       <c r="K42" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N42" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -3923,16 +3932,16 @@
         <v>23</v>
       </c>
       <c r="H43" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I43" t="s">
         <v>427</v>
       </c>
       <c r="K43" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N43" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -3952,16 +3961,16 @@
         <v>23</v>
       </c>
       <c r="H44" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I44" t="s">
         <v>427</v>
       </c>
       <c r="K44" t="s">
+        <v>485</v>
+      </c>
+      <c r="N44" t="s">
         <v>487</v>
-      </c>
-      <c r="N44" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -3981,16 +3990,16 @@
         <v>23</v>
       </c>
       <c r="H45" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I45" t="s">
         <v>427</v>
       </c>
       <c r="K45" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N45" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -4010,16 +4019,16 @@
         <v>23</v>
       </c>
       <c r="H46" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I46" t="s">
         <v>427</v>
       </c>
       <c r="K46" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N46" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -4039,16 +4048,16 @@
         <v>23</v>
       </c>
       <c r="H47" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I47" t="s">
         <v>427</v>
       </c>
       <c r="K47" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N47" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -4068,16 +4077,16 @@
         <v>23</v>
       </c>
       <c r="H48" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I48" t="s">
         <v>427</v>
       </c>
       <c r="K48" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N48" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.25">
@@ -4097,16 +4106,16 @@
         <v>23</v>
       </c>
       <c r="H49" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I49" t="s">
         <v>427</v>
       </c>
       <c r="K49" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N49" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.25">
@@ -4126,16 +4135,16 @@
         <v>23</v>
       </c>
       <c r="H50" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I50" t="s">
         <v>427</v>
       </c>
       <c r="K50" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N50" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="51" spans="2:19" x14ac:dyDescent="0.25">
@@ -4155,16 +4164,16 @@
         <v>23</v>
       </c>
       <c r="H51" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I51" t="s">
         <v>427</v>
       </c>
       <c r="K51" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N51" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.25">
@@ -4184,16 +4193,16 @@
         <v>23</v>
       </c>
       <c r="H52" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I52" t="s">
         <v>427</v>
       </c>
       <c r="K52" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N52" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.25">
@@ -4213,16 +4222,16 @@
         <v>23</v>
       </c>
       <c r="H53" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I53" t="s">
         <v>427</v>
       </c>
       <c r="K53" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N53" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.25">
@@ -4242,16 +4251,16 @@
         <v>23</v>
       </c>
       <c r="H54" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I54" t="s">
         <v>427</v>
       </c>
       <c r="K54" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N54" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.25">
@@ -4271,16 +4280,16 @@
         <v>23</v>
       </c>
       <c r="H55" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I55" t="s">
         <v>427</v>
       </c>
       <c r="K55" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N55" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.25">
@@ -4300,16 +4309,16 @@
         <v>23</v>
       </c>
       <c r="H56" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I56" t="s">
         <v>427</v>
       </c>
       <c r="K56" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="N56" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
@@ -4329,7 +4338,7 @@
         <v>32</v>
       </c>
       <c r="H57" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="I57" t="s">
         <v>427</v>
@@ -4355,7 +4364,7 @@
         <v>32</v>
       </c>
       <c r="H58" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="I58" t="s">
         <v>427</v>
@@ -4381,16 +4390,16 @@
         <v>49</v>
       </c>
       <c r="H59" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I59" t="s">
         <v>414</v>
       </c>
       <c r="N59" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="S59" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="60" spans="2:19" x14ac:dyDescent="0.25">
@@ -4410,16 +4419,16 @@
         <v>49</v>
       </c>
       <c r="H60" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I60" t="s">
         <v>414</v>
       </c>
       <c r="N60" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="S60" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
@@ -4439,13 +4448,13 @@
         <v>49</v>
       </c>
       <c r="H61" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I61" t="s">
         <v>414</v>
       </c>
       <c r="N61" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="S61" t="s">
         <v>440</v>
@@ -4468,16 +4477,16 @@
         <v>49</v>
       </c>
       <c r="H62" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I62" t="s">
         <v>414</v>
       </c>
       <c r="N62" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="S62" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
@@ -4497,16 +4506,16 @@
         <v>49</v>
       </c>
       <c r="H63" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I63" t="s">
         <v>414</v>
       </c>
       <c r="N63" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="S63" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="64" spans="2:19" x14ac:dyDescent="0.25">
@@ -4526,13 +4535,13 @@
         <v>49</v>
       </c>
       <c r="H64" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I64" t="s">
         <v>414</v>
       </c>
       <c r="N64" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="S64" t="s">
         <v>440</v>
@@ -4555,16 +4564,16 @@
         <v>49</v>
       </c>
       <c r="H65" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I65" t="s">
         <v>414</v>
       </c>
       <c r="N65" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="S65" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="66" spans="2:19" x14ac:dyDescent="0.25">
@@ -4584,16 +4593,16 @@
         <v>49</v>
       </c>
       <c r="H66" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I66" t="s">
         <v>414</v>
       </c>
       <c r="N66" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="S66" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.25">
@@ -4613,13 +4622,13 @@
         <v>49</v>
       </c>
       <c r="H67" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I67" t="s">
         <v>414</v>
       </c>
       <c r="N67" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="S67" t="s">
         <v>440</v>
@@ -4642,10 +4651,10 @@
         <v>57</v>
       </c>
       <c r="H68" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="I68" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="J68">
         <v>6</v>
@@ -4668,10 +4677,10 @@
         <v>57</v>
       </c>
       <c r="H69" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="I69" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="J69">
         <v>6</v>
@@ -4694,10 +4703,10 @@
         <v>58</v>
       </c>
       <c r="H70" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="I70" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="J70">
         <v>3</v>
@@ -4720,10 +4729,10 @@
         <v>58</v>
       </c>
       <c r="H71" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="I71" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="J71">
         <v>3</v>
@@ -4746,10 +4755,10 @@
         <v>60</v>
       </c>
       <c r="H72" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="I72" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J72">
         <v>3</v>
@@ -4772,10 +4781,10 @@
         <v>60</v>
       </c>
       <c r="H73" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="I73" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="J73">
         <v>3</v>
@@ -4824,10 +4833,10 @@
         <v>61</v>
       </c>
       <c r="H75" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="I75" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="J75">
         <v>6</v>
@@ -4853,7 +4862,7 @@
         <v>430</v>
       </c>
       <c r="I76" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J76">
         <v>3</v>
@@ -4876,10 +4885,10 @@
         <v>61</v>
       </c>
       <c r="H77" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="I77" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="J77">
         <v>6</v>
@@ -4902,7 +4911,7 @@
         <v>61</v>
       </c>
       <c r="H78" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="I78" t="s">
         <v>441</v>
@@ -4931,7 +4940,7 @@
         <v>443</v>
       </c>
       <c r="I79" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="J79">
         <v>6</v>
@@ -4957,7 +4966,7 @@
         <v>431</v>
       </c>
       <c r="I80" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="J80">
         <v>3</v>
@@ -4980,10 +4989,10 @@
         <v>61</v>
       </c>
       <c r="H81" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="I81" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="J81">
         <v>6</v>
@@ -5006,7 +5015,7 @@
         <v>64</v>
       </c>
       <c r="H82" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="I82" t="s">
         <v>414</v>
@@ -5029,10 +5038,10 @@
         <v>64</v>
       </c>
       <c r="H83" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="I83" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J83">
         <v>3</v>
@@ -5055,7 +5064,7 @@
         <v>64</v>
       </c>
       <c r="H84" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="I84" t="s">
         <v>414</v>
@@ -5078,10 +5087,10 @@
         <v>64</v>
       </c>
       <c r="H85" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="I85" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J85">
         <v>3</v>
@@ -5104,7 +5113,7 @@
         <v>64</v>
       </c>
       <c r="H86" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="I86" t="s">
         <v>414</v>
@@ -5112,7 +5121,7 @@
     </row>
     <row r="87" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>204</v>
@@ -5130,10 +5139,10 @@
         <v>64</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J87" s="1">
         <v>3</v>
@@ -5156,7 +5165,7 @@
         <v>64</v>
       </c>
       <c r="H88" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="I88" t="s">
         <v>414</v>
@@ -5179,10 +5188,10 @@
         <v>64</v>
       </c>
       <c r="H89" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="I89" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="J89">
         <v>3</v>
@@ -5205,10 +5214,10 @@
         <v>65</v>
       </c>
       <c r="H90" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="I90" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.25">
@@ -5228,10 +5237,10 @@
         <v>65</v>
       </c>
       <c r="H91" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="I91" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.25">
@@ -5251,10 +5260,10 @@
         <v>65</v>
       </c>
       <c r="H92" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="I92" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.25">
@@ -5274,10 +5283,10 @@
         <v>65</v>
       </c>
       <c r="H93" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="I93" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.25">
@@ -5297,10 +5306,10 @@
         <v>65</v>
       </c>
       <c r="H94" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="I94" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.25">
@@ -5320,13 +5329,13 @@
         <v>66</v>
       </c>
       <c r="H95" t="s">
+        <v>530</v>
+      </c>
+      <c r="I95" t="s">
         <v>532</v>
       </c>
-      <c r="I95" t="s">
-        <v>534</v>
-      </c>
       <c r="M95" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="S95" t="s">
         <v>440</v>
@@ -5349,16 +5358,16 @@
         <v>66</v>
       </c>
       <c r="H96" t="s">
+        <v>530</v>
+      </c>
+      <c r="I96" t="s">
         <v>532</v>
       </c>
-      <c r="I96" t="s">
-        <v>534</v>
-      </c>
       <c r="M96" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="S96" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
@@ -5378,13 +5387,13 @@
         <v>66</v>
       </c>
       <c r="H97" t="s">
+        <v>530</v>
+      </c>
+      <c r="I97" t="s">
         <v>532</v>
       </c>
-      <c r="I97" t="s">
+      <c r="M97" t="s">
         <v>534</v>
-      </c>
-      <c r="M97" t="s">
-        <v>536</v>
       </c>
       <c r="S97" t="s">
         <v>440</v>
@@ -5407,16 +5416,16 @@
         <v>66</v>
       </c>
       <c r="H98" t="s">
+        <v>530</v>
+      </c>
+      <c r="I98" t="s">
         <v>532</v>
       </c>
-      <c r="I98" t="s">
+      <c r="M98" t="s">
         <v>534</v>
       </c>
-      <c r="M98" t="s">
-        <v>536</v>
-      </c>
       <c r="S98" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
@@ -5436,13 +5445,13 @@
         <v>66</v>
       </c>
       <c r="H99" t="s">
+        <v>530</v>
+      </c>
+      <c r="I99" t="s">
         <v>532</v>
       </c>
-      <c r="I99" t="s">
-        <v>534</v>
-      </c>
       <c r="M99" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="S99" t="s">
         <v>440</v>
@@ -5465,16 +5474,16 @@
         <v>66</v>
       </c>
       <c r="H100" t="s">
+        <v>530</v>
+      </c>
+      <c r="I100" t="s">
         <v>532</v>
       </c>
-      <c r="I100" t="s">
-        <v>534</v>
-      </c>
       <c r="M100" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="S100" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.25">
@@ -5494,10 +5503,10 @@
         <v>66</v>
       </c>
       <c r="H101" t="s">
+        <v>530</v>
+      </c>
+      <c r="I101" t="s">
         <v>532</v>
-      </c>
-      <c r="I101" t="s">
-        <v>534</v>
       </c>
       <c r="M101" t="s">
         <v>421</v>
@@ -5523,7 +5532,7 @@
         <v>67</v>
       </c>
       <c r="H102" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="I102" t="s">
         <v>423</v>
@@ -5546,7 +5555,7 @@
         <v>67</v>
       </c>
       <c r="H103" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I103" t="s">
         <v>423</v>
@@ -5569,15 +5578,15 @@
         <v>67</v>
       </c>
       <c r="H104" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="I104" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
     </row>
     <row r="105" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>202</v>
@@ -5598,7 +5607,7 @@
         <v>68</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>432</v>
@@ -5609,7 +5618,7 @@
     </row>
     <row r="106" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>96</v>
@@ -5630,7 +5639,7 @@
         <v>68</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>432</v>
@@ -5641,7 +5650,7 @@
     </row>
     <row r="107" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>120</v>
@@ -5662,7 +5671,7 @@
         <v>68</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>432</v>
@@ -5673,7 +5682,7 @@
     </row>
     <row r="108" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>216</v>
@@ -5691,7 +5700,7 @@
         <v>74</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>432</v>
@@ -5702,7 +5711,7 @@
     </row>
     <row r="109" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>214</v>
@@ -5720,7 +5729,7 @@
         <v>74</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>432</v>
@@ -5731,7 +5740,7 @@
     </row>
     <row r="110" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>32</v>
@@ -5760,7 +5769,7 @@
     </row>
     <row r="111" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>92</v>
@@ -5781,15 +5790,15 @@
         <v>75</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="112" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>94</v>
@@ -5810,10 +5819,10 @@
         <v>75</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
@@ -5841,7 +5850,7 @@
       <c r="J113">
         <v>6</v>
       </c>
-      <c r="K113" t="s">
+      <c r="P113" t="s">
         <v>448</v>
       </c>
     </row>
@@ -5870,7 +5879,7 @@
       <c r="J114">
         <v>6</v>
       </c>
-      <c r="K114" t="s">
+      <c r="P114" t="s">
         <v>449</v>
       </c>
     </row>
@@ -5891,12 +5900,12 @@
         <v>77</v>
       </c>
       <c r="H115" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="I115" t="s">
-        <v>561</v>
-      </c>
-      <c r="K115" t="s">
+        <v>558</v>
+      </c>
+      <c r="P115" t="s">
         <v>421</v>
       </c>
     </row>
@@ -5925,7 +5934,7 @@
       <c r="J116">
         <v>6</v>
       </c>
-      <c r="K116" t="s">
+      <c r="P116" t="s">
         <v>421</v>
       </c>
     </row>
@@ -5946,7 +5955,7 @@
         <v>78</v>
       </c>
       <c r="H117" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I117" t="s">
         <v>423</v>
@@ -5954,7 +5963,7 @@
     </row>
     <row r="118" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>353</v>
@@ -5972,10 +5981,10 @@
         <v>78</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="S118" s="1" t="s">
         <v>440</v>
@@ -5983,7 +5992,7 @@
     </row>
     <row r="119" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>349</v>
@@ -6001,7 +6010,7 @@
         <v>78</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>423</v>
@@ -6012,7 +6021,7 @@
     </row>
     <row r="120" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>357</v>
@@ -6030,18 +6039,18 @@
         <v>78</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="S120" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="121" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>355</v>
@@ -6059,18 +6068,18 @@
         <v>78</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="S121" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="122" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>361</v>
@@ -6088,7 +6097,7 @@
         <v>78</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>423</v>
@@ -6096,7 +6105,7 @@
     </row>
     <row r="123" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>363</v>
@@ -6114,7 +6123,7 @@
         <v>78</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>423</v>
@@ -6122,7 +6131,7 @@
     </row>
     <row r="124" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>351</v>
@@ -6140,7 +6149,7 @@
         <v>78</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>423</v>
@@ -6148,7 +6157,7 @@
     </row>
     <row r="125" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>154</v>
@@ -6169,15 +6178,15 @@
         <v>83</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>547</v>
+        <v>617</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
     </row>
     <row r="126" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>156</v>
@@ -6198,15 +6207,15 @@
         <v>83</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>547</v>
+        <v>619</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>564</v>
+        <v>618</v>
       </c>
     </row>
     <row r="127" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>152</v>
@@ -6227,7 +6236,7 @@
         <v>83</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I127" s="1" t="s">
         <v>423</v>
@@ -6238,7 +6247,7 @@
     </row>
     <row r="128" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>172</v>
@@ -6256,7 +6265,7 @@
         <v>83</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>414</v>
@@ -6267,7 +6276,7 @@
     </row>
     <row r="129" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>174</v>
@@ -6285,7 +6294,7 @@
         <v>83</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>414</v>
@@ -6296,7 +6305,7 @@
     </row>
     <row r="130" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>170</v>
@@ -6314,10 +6323,10 @@
         <v>83</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>548</v>
+        <v>620</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="Q130" s="1" t="s">
         <v>419</v>
@@ -6637,7 +6646,7 @@
     </row>
     <row r="143" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>38</v>
@@ -6666,7 +6675,7 @@
     </row>
     <row r="144" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>40</v>
@@ -6695,7 +6704,7 @@
     </row>
     <row r="145" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>212</v>
@@ -6718,7 +6727,7 @@
     </row>
     <row r="146" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>208</v>
@@ -6736,7 +6745,7 @@
         <v>89</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>423</v>
@@ -6750,7 +6759,7 @@
     </row>
     <row r="147" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>88</v>
@@ -6768,7 +6777,7 @@
         <v>89</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>423</v>
@@ -6777,12 +6786,12 @@
         <v>6</v>
       </c>
       <c r="S147" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="148" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>90</v>
@@ -6800,7 +6809,7 @@
         <v>89</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>423</v>
@@ -6809,12 +6818,12 @@
         <v>6</v>
       </c>
       <c r="S148" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="149" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>42</v>
@@ -6840,7 +6849,7 @@
     </row>
     <row r="150" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>210</v>
@@ -6858,10 +6867,10 @@
         <v>89</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="J150" s="1">
         <v>3</v>
@@ -6884,13 +6893,13 @@
         <v>94</v>
       </c>
       <c r="H151" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="I151" t="s">
         <v>414</v>
       </c>
       <c r="S151" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="152" spans="1:19" x14ac:dyDescent="0.25">
@@ -6910,13 +6919,13 @@
         <v>94</v>
       </c>
       <c r="H152" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="I152" t="s">
         <v>414</v>
       </c>
       <c r="S152" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="153" spans="1:19" x14ac:dyDescent="0.25">
@@ -6936,7 +6945,7 @@
         <v>94</v>
       </c>
       <c r="H153" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="I153" t="s">
         <v>414</v>
@@ -6962,13 +6971,13 @@
         <v>94</v>
       </c>
       <c r="H154" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="I154" t="s">
         <v>414</v>
       </c>
       <c r="S154" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="155" spans="1:19" x14ac:dyDescent="0.25">
@@ -6988,13 +6997,13 @@
         <v>94</v>
       </c>
       <c r="H155" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="I155" t="s">
         <v>414</v>
       </c>
       <c r="S155" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="156" spans="1:19" x14ac:dyDescent="0.25">
@@ -7014,7 +7023,7 @@
         <v>94</v>
       </c>
       <c r="H156" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="I156" t="s">
         <v>414</v>
@@ -7025,7 +7034,7 @@
     </row>
     <row r="157" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>341</v>
@@ -7043,7 +7052,7 @@
         <v>98</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="I157" s="1" t="s">
         <v>427</v>
@@ -7051,7 +7060,7 @@
     </row>
     <row r="158" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>343</v>
@@ -7069,7 +7078,7 @@
         <v>98</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="I158" s="1" t="s">
         <v>427</v>
@@ -7092,10 +7101,10 @@
         <v>103</v>
       </c>
       <c r="H159" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="I159" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="160" spans="1:19" x14ac:dyDescent="0.25">
@@ -7115,7 +7124,7 @@
         <v>103</v>
       </c>
       <c r="H160" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="I160" t="s">
         <v>432</v>
@@ -7141,10 +7150,10 @@
         <v>104</v>
       </c>
       <c r="H161" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="I161" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="162" spans="2:20" x14ac:dyDescent="0.25">
@@ -7164,10 +7173,10 @@
         <v>104</v>
       </c>
       <c r="H162" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="I162" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="163" spans="2:20" x14ac:dyDescent="0.25">
@@ -7187,10 +7196,10 @@
         <v>104</v>
       </c>
       <c r="H163" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="I163" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="164" spans="2:20" x14ac:dyDescent="0.25">
@@ -7210,13 +7219,13 @@
         <v>104</v>
       </c>
       <c r="H164" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="I164" t="s">
         <v>414</v>
       </c>
       <c r="S164" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="165" spans="2:20" x14ac:dyDescent="0.25">
@@ -7236,13 +7245,13 @@
         <v>104</v>
       </c>
       <c r="H165" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="I165" t="s">
         <v>414</v>
       </c>
       <c r="S165" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="166" spans="2:20" x14ac:dyDescent="0.25">
@@ -7262,10 +7271,10 @@
         <v>104</v>
       </c>
       <c r="H166" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="I166" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="167" spans="2:20" x14ac:dyDescent="0.25">
@@ -7285,10 +7294,10 @@
         <v>104</v>
       </c>
       <c r="H167" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="I167" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="168" spans="2:20" x14ac:dyDescent="0.25">
@@ -7308,10 +7317,10 @@
         <v>104</v>
       </c>
       <c r="H168" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="I168" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
     </row>
     <row r="169" spans="2:20" x14ac:dyDescent="0.25">
@@ -7322,7 +7331,7 @@
         <v>1491</v>
       </c>
       <c r="E169" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="F169">
         <v>18</v>
@@ -7331,7 +7340,7 @@
         <v>106</v>
       </c>
       <c r="H169" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="I169" t="s">
         <v>414</v>
@@ -7354,7 +7363,7 @@
         <v>107</v>
       </c>
       <c r="H170" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="I170" t="s">
         <v>423</v>
@@ -7377,10 +7386,10 @@
         <v>107</v>
       </c>
       <c r="H171" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="I171" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
     </row>
     <row r="172" spans="2:20" x14ac:dyDescent="0.25">
@@ -7400,13 +7409,13 @@
         <v>109</v>
       </c>
       <c r="H172" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="I172" t="s">
         <v>414</v>
       </c>
       <c r="L172" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
     </row>
     <row r="173" spans="2:20" x14ac:dyDescent="0.25">
@@ -7426,13 +7435,13 @@
         <v>109</v>
       </c>
       <c r="H173" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="I173" t="s">
         <v>414</v>
       </c>
       <c r="L173" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="174" spans="2:20" x14ac:dyDescent="0.25">
@@ -7452,13 +7461,13 @@
         <v>109</v>
       </c>
       <c r="H174" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="I174" t="s">
         <v>414</v>
       </c>
       <c r="L174" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
     </row>
     <row r="175" spans="2:20" x14ac:dyDescent="0.25">
@@ -7478,16 +7487,16 @@
         <v>109</v>
       </c>
       <c r="H175" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="I175" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="L175" t="s">
         <v>445</v>
       </c>
       <c r="T175" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
     </row>
     <row r="176" spans="2:20" x14ac:dyDescent="0.25">
@@ -7507,10 +7516,10 @@
         <v>109</v>
       </c>
       <c r="H176" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="I176" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="L176" t="s">
         <v>445</v>
@@ -7536,10 +7545,10 @@
         <v>109</v>
       </c>
       <c r="H177" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="I177" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="L177" t="s">
         <v>445</v>
@@ -7565,10 +7574,10 @@
         <v>109</v>
       </c>
       <c r="H178" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="I178" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="L178" t="s">
         <v>445</v>
@@ -7594,10 +7603,10 @@
         <v>109</v>
       </c>
       <c r="H179" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="I179" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="L179" t="s">
         <v>445</v>
@@ -7623,10 +7632,10 @@
         <v>109</v>
       </c>
       <c r="H180" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="I180" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="L180" t="s">
         <v>445</v>
@@ -7652,10 +7661,10 @@
         <v>115</v>
       </c>
       <c r="H181" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="I181" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="T181" t="s">
         <v>451</v>
@@ -7678,10 +7687,10 @@
         <v>115</v>
       </c>
       <c r="H182" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="I182" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="T182" t="s">
         <v>452</v>
@@ -7704,10 +7713,10 @@
         <v>115</v>
       </c>
       <c r="H183" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="I183" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="T183" t="s">
         <v>453</v>
@@ -7730,7 +7739,7 @@
         <v>116</v>
       </c>
       <c r="H184" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="I184" t="s">
         <v>432</v>
@@ -7759,7 +7768,7 @@
         <v>116</v>
       </c>
       <c r="H185" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="I185" t="s">
         <v>423</v>
@@ -7785,10 +7794,10 @@
         <v>117</v>
       </c>
       <c r="H186" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="I186" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
     </row>
     <row r="187" spans="2:20" x14ac:dyDescent="0.25">
@@ -7808,10 +7817,10 @@
         <v>117</v>
       </c>
       <c r="H187" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="I187" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
     </row>
     <row r="188" spans="2:20" x14ac:dyDescent="0.25">
@@ -7834,7 +7843,7 @@
         <v>134</v>
       </c>
       <c r="H188" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="I188" t="s">
         <v>414</v>
@@ -7857,10 +7866,10 @@
         <v>135</v>
       </c>
       <c r="H189" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="I189" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="T189" t="s">
         <v>451</v>
@@ -7883,10 +7892,10 @@
         <v>135</v>
       </c>
       <c r="H190" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="I190" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="T190" t="s">
         <v>452</v>
@@ -7909,10 +7918,10 @@
         <v>135</v>
       </c>
       <c r="H191" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="I191" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="T191" t="s">
         <v>453</v>
@@ -7935,7 +7944,7 @@
         <v>135</v>
       </c>
       <c r="H192" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="I192" t="s">
         <v>423</v>
@@ -7961,7 +7970,7 @@
         <v>135</v>
       </c>
       <c r="H193" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="I193" t="s">
         <v>423</v>
@@ -7987,7 +7996,7 @@
         <v>135</v>
       </c>
       <c r="H194" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="I194" t="s">
         <v>423</v>
@@ -8013,13 +8022,13 @@
         <v>151</v>
       </c>
       <c r="H195" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I195" t="s">
         <v>423</v>
       </c>
       <c r="M195" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="196" spans="2:20" x14ac:dyDescent="0.25">
@@ -8039,13 +8048,13 @@
         <v>151</v>
       </c>
       <c r="H196" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="I196" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="M196" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
     </row>
     <row r="197" spans="2:20" x14ac:dyDescent="0.25">
@@ -8065,13 +8074,13 @@
         <v>151</v>
       </c>
       <c r="H197" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I197" t="s">
         <v>423</v>
       </c>
       <c r="M197" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="198" spans="2:20" x14ac:dyDescent="0.25">
@@ -8091,13 +8100,13 @@
         <v>151</v>
       </c>
       <c r="H198" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="I198" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="M198" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="199" spans="2:20" x14ac:dyDescent="0.25">
@@ -8117,13 +8126,13 @@
         <v>151</v>
       </c>
       <c r="H199" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I199" t="s">
         <v>423</v>
       </c>
       <c r="M199" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="200" spans="2:20" x14ac:dyDescent="0.25">
@@ -8143,13 +8152,13 @@
         <v>151</v>
       </c>
       <c r="H200" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="I200" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="M200" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
     </row>
     <row r="201" spans="2:20" x14ac:dyDescent="0.25">
@@ -8169,13 +8178,13 @@
         <v>151</v>
       </c>
       <c r="H201" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="I201" t="s">
         <v>423</v>
       </c>
       <c r="M201" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="202" spans="2:20" x14ac:dyDescent="0.25">
@@ -8195,13 +8204,13 @@
         <v>151</v>
       </c>
       <c r="H202" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="I202" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="M202" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
     </row>
     <row r="203" spans="2:20" x14ac:dyDescent="0.25">
@@ -8221,10 +8230,10 @@
         <v>152</v>
       </c>
       <c r="H203" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="I203" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="J203">
         <v>3</v>
@@ -8247,10 +8256,10 @@
         <v>152</v>
       </c>
       <c r="H204" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="I204" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
     </row>
   </sheetData>

</xml_diff>